<commit_message>
191210 | Github API
</commit_message>
<xml_diff>
--- a/[계절학기] 191209_학습계획서_대전_1반_김기은.xlsx
+++ b/[계절학기] 191209_학습계획서_대전_1반_김기은.xlsx
@@ -4,20 +4,21 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="날짜별 계획 " sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="실적(daily) 양식 (데일리별로 신규로 작성할 것)" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="실적(daily) 19.12.09" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="실적(daily) 19.12.10" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mg/+Uanbnj0WK4sMUtCChXBfyek6Q=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mgYvj+F9v3W6t2MsNxKEMJdnxX0Rg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>자기주도학습 계획표</t>
   </si>
@@ -28,39 +29,54 @@
     <t>학습 형태</t>
   </si>
   <si>
-    <t xml:space="preserve">□ 개별   □ 2인 1조   □ 팀별 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 개별</t>
   </si>
   <si>
+    <t>개별</t>
+  </si>
+  <si>
     <t>구성원</t>
   </si>
   <si>
+    <t>김기은</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 김기은</t>
+  </si>
+  <si>
     <t>일정</t>
   </si>
   <si>
+    <t>2019.12.09</t>
+  </si>
+  <si>
+    <t>2019.12.10.</t>
+  </si>
+  <si>
     <t>데일리 목표</t>
   </si>
   <si>
-    <t xml:space="preserve"> 김기은</t>
+    <t>자기주도학습 계획 작성</t>
   </si>
   <si>
     <t>12/09(월)</t>
   </si>
   <si>
+    <t>DataBase</t>
+  </si>
+  <si>
+    <t>12/10(화)</t>
+  </si>
+  <si>
+    <t>12/11(수)</t>
+  </si>
+  <si>
+    <t>12/16(월)</t>
+  </si>
+  <si>
     <t>주요 내용 요약</t>
   </si>
   <si>
-    <t>12/10(화)</t>
-  </si>
-  <si>
-    <t>12/11(수)</t>
-  </si>
-  <si>
-    <t>12/16(월)</t>
-  </si>
-  <si>
     <t>12/17(화)</t>
   </si>
   <si>
@@ -68,6 +84,9 @@
   </si>
   <si>
     <t>12/19(목)</t>
+  </si>
+  <si>
+    <t>- Github API에서 레포지토리 데이터 추출 및 Python을 이용하여 원하는 API 재가공</t>
   </si>
   <si>
     <t xml:space="preserve"> - 자기주도학습 계획 작성</t>
@@ -93,6 +112,9 @@
 (분야 및 키워드) </t>
   </si>
   <si>
+    <t xml:space="preserve"> - 지난 1학기 동안 배운 내용을 보기 좋게 포트폴리오로 작성하는 것을 목표로 하여 계획서를 작성</t>
+  </si>
+  <si>
     <t>- 자기 주도학습 계획 작성</t>
   </si>
   <si>
@@ -143,13 +165,18 @@
   </si>
   <si>
     <t>실행 내용</t>
+  </si>
+  <si>
+    <t>- Github API에서 레포지토리
+데이터 추출 및 Python을 이용하여
+원하는 API 재가공</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -168,17 +195,8 @@
     <font/>
     <font>
       <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Malgun Gothic"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Malgun Gothic"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -308,6 +326,20 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -331,20 +363,6 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -495,7 +513,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
@@ -503,43 +524,40 @@
     <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -563,7 +581,7 @@
     <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -594,6 +612,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -824,106 +846,106 @@
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
+      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" ht="16.5" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
+      <c r="C4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" ht="21.75" customHeight="1">
       <c r="B5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="13" t="s">
+      <c r="D5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="E5" s="10" t="s">
         <v>16</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" ht="39.75" customHeight="1">
       <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>22</v>
+        <v>11</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" ht="39.75" customHeight="1">
       <c r="B7" s="19" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" ht="39.75" customHeight="1">
@@ -958,36 +980,38 @@
     </row>
     <row r="11" ht="143.25" customHeight="1">
       <c r="B11" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="11"/>
+        <v>38</v>
+      </c>
+      <c r="C11" s="10"/>
       <c r="D11" s="29" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" ht="39.75" customHeight="1">
       <c r="B12" s="28" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="30"/>
+        <v>31</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>46</v>
+      </c>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
       <c r="G12" s="30"/>
@@ -2011,24 +2035,24 @@
     <row r="1000" ht="16.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="I7:I10"/>
     <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C12:C15"/>
     <mergeCell ref="D12:D15"/>
     <mergeCell ref="E12:E15"/>
     <mergeCell ref="F12:F15"/>
     <mergeCell ref="G12:G15"/>
     <mergeCell ref="H12:H15"/>
-    <mergeCell ref="C12:C15"/>
     <mergeCell ref="I12:I15"/>
-    <mergeCell ref="I7:I10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="H7:H10"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="C3:I3"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="C7:C10"/>
     <mergeCell ref="D7:D10"/>
-    <mergeCell ref="F7:F10"/>
     <mergeCell ref="E7:E10"/>
   </mergeCells>
   <printOptions/>
@@ -2096,43 +2120,1164 @@
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" ht="27.75" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
+      <c r="C4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" ht="27.75" customHeight="1">
       <c r="B5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" ht="27.75" customHeight="1">
       <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8"/>
+        <v>11</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" ht="372.0" customHeight="1">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
+    </row>
+    <row r="8" ht="16.5" customHeight="1"/>
+    <row r="9" ht="16.5" customHeight="1"/>
+    <row r="10" ht="16.5" customHeight="1"/>
+    <row r="11" ht="16.5" customHeight="1"/>
+    <row r="12" ht="16.5" customHeight="1"/>
+    <row r="13" ht="16.5" customHeight="1"/>
+    <row r="14" ht="16.5" customHeight="1"/>
+    <row r="15" ht="16.5" customHeight="1"/>
+    <row r="16" ht="16.5" customHeight="1"/>
+    <row r="17" ht="16.5" customHeight="1"/>
+    <row r="18" ht="16.5" customHeight="1"/>
+    <row r="19" ht="16.5" customHeight="1"/>
+    <row r="20" ht="16.5" customHeight="1"/>
+    <row r="21" ht="16.5" customHeight="1"/>
+    <row r="22" ht="16.5" customHeight="1"/>
+    <row r="23" ht="16.5" customHeight="1"/>
+    <row r="24" ht="16.5" customHeight="1"/>
+    <row r="25" ht="16.5" customHeight="1"/>
+    <row r="26" ht="16.5" customHeight="1"/>
+    <row r="27" ht="16.5" customHeight="1"/>
+    <row r="28" ht="16.5" customHeight="1"/>
+    <row r="29" ht="16.5" customHeight="1"/>
+    <row r="30" ht="16.5" customHeight="1"/>
+    <row r="31" ht="16.5" customHeight="1"/>
+    <row r="32" ht="16.5" customHeight="1"/>
+    <row r="33" ht="16.5" customHeight="1"/>
+    <row r="34" ht="16.5" customHeight="1"/>
+    <row r="35" ht="16.5" customHeight="1"/>
+    <row r="36" ht="16.5" customHeight="1"/>
+    <row r="37" ht="16.5" customHeight="1"/>
+    <row r="38" ht="16.5" customHeight="1"/>
+    <row r="39" ht="16.5" customHeight="1"/>
+    <row r="40" ht="16.5" customHeight="1"/>
+    <row r="41" ht="16.5" customHeight="1"/>
+    <row r="42" ht="16.5" customHeight="1"/>
+    <row r="43" ht="16.5" customHeight="1"/>
+    <row r="44" ht="16.5" customHeight="1"/>
+    <row r="45" ht="16.5" customHeight="1"/>
+    <row r="46" ht="16.5" customHeight="1"/>
+    <row r="47" ht="16.5" customHeight="1"/>
+    <row r="48" ht="16.5" customHeight="1"/>
+    <row r="49" ht="16.5" customHeight="1"/>
+    <row r="50" ht="16.5" customHeight="1"/>
+    <row r="51" ht="16.5" customHeight="1"/>
+    <row r="52" ht="16.5" customHeight="1"/>
+    <row r="53" ht="16.5" customHeight="1"/>
+    <row r="54" ht="16.5" customHeight="1"/>
+    <row r="55" ht="16.5" customHeight="1"/>
+    <row r="56" ht="16.5" customHeight="1"/>
+    <row r="57" ht="16.5" customHeight="1"/>
+    <row r="58" ht="16.5" customHeight="1"/>
+    <row r="59" ht="16.5" customHeight="1"/>
+    <row r="60" ht="16.5" customHeight="1"/>
+    <row r="61" ht="16.5" customHeight="1"/>
+    <row r="62" ht="16.5" customHeight="1"/>
+    <row r="63" ht="16.5" customHeight="1"/>
+    <row r="64" ht="16.5" customHeight="1"/>
+    <row r="65" ht="16.5" customHeight="1"/>
+    <row r="66" ht="16.5" customHeight="1"/>
+    <row r="67" ht="16.5" customHeight="1"/>
+    <row r="68" ht="16.5" customHeight="1"/>
+    <row r="69" ht="16.5" customHeight="1"/>
+    <row r="70" ht="16.5" customHeight="1"/>
+    <row r="71" ht="16.5" customHeight="1"/>
+    <row r="72" ht="16.5" customHeight="1"/>
+    <row r="73" ht="16.5" customHeight="1"/>
+    <row r="74" ht="16.5" customHeight="1"/>
+    <row r="75" ht="16.5" customHeight="1"/>
+    <row r="76" ht="16.5" customHeight="1"/>
+    <row r="77" ht="16.5" customHeight="1"/>
+    <row r="78" ht="16.5" customHeight="1"/>
+    <row r="79" ht="16.5" customHeight="1"/>
+    <row r="80" ht="16.5" customHeight="1"/>
+    <row r="81" ht="16.5" customHeight="1"/>
+    <row r="82" ht="16.5" customHeight="1"/>
+    <row r="83" ht="16.5" customHeight="1"/>
+    <row r="84" ht="16.5" customHeight="1"/>
+    <row r="85" ht="16.5" customHeight="1"/>
+    <row r="86" ht="16.5" customHeight="1"/>
+    <row r="87" ht="16.5" customHeight="1"/>
+    <row r="88" ht="16.5" customHeight="1"/>
+    <row r="89" ht="16.5" customHeight="1"/>
+    <row r="90" ht="16.5" customHeight="1"/>
+    <row r="91" ht="16.5" customHeight="1"/>
+    <row r="92" ht="16.5" customHeight="1"/>
+    <row r="93" ht="16.5" customHeight="1"/>
+    <row r="94" ht="16.5" customHeight="1"/>
+    <row r="95" ht="16.5" customHeight="1"/>
+    <row r="96" ht="16.5" customHeight="1"/>
+    <row r="97" ht="16.5" customHeight="1"/>
+    <row r="98" ht="16.5" customHeight="1"/>
+    <row r="99" ht="16.5" customHeight="1"/>
+    <row r="100" ht="16.5" customHeight="1"/>
+    <row r="101" ht="16.5" customHeight="1"/>
+    <row r="102" ht="16.5" customHeight="1"/>
+    <row r="103" ht="16.5" customHeight="1"/>
+    <row r="104" ht="16.5" customHeight="1"/>
+    <row r="105" ht="16.5" customHeight="1"/>
+    <row r="106" ht="16.5" customHeight="1"/>
+    <row r="107" ht="16.5" customHeight="1"/>
+    <row r="108" ht="16.5" customHeight="1"/>
+    <row r="109" ht="16.5" customHeight="1"/>
+    <row r="110" ht="16.5" customHeight="1"/>
+    <row r="111" ht="16.5" customHeight="1"/>
+    <row r="112" ht="16.5" customHeight="1"/>
+    <row r="113" ht="16.5" customHeight="1"/>
+    <row r="114" ht="16.5" customHeight="1"/>
+    <row r="115" ht="16.5" customHeight="1"/>
+    <row r="116" ht="16.5" customHeight="1"/>
+    <row r="117" ht="16.5" customHeight="1"/>
+    <row r="118" ht="16.5" customHeight="1"/>
+    <row r="119" ht="16.5" customHeight="1"/>
+    <row r="120" ht="16.5" customHeight="1"/>
+    <row r="121" ht="16.5" customHeight="1"/>
+    <row r="122" ht="16.5" customHeight="1"/>
+    <row r="123" ht="16.5" customHeight="1"/>
+    <row r="124" ht="16.5" customHeight="1"/>
+    <row r="125" ht="16.5" customHeight="1"/>
+    <row r="126" ht="16.5" customHeight="1"/>
+    <row r="127" ht="16.5" customHeight="1"/>
+    <row r="128" ht="16.5" customHeight="1"/>
+    <row r="129" ht="16.5" customHeight="1"/>
+    <row r="130" ht="16.5" customHeight="1"/>
+    <row r="131" ht="16.5" customHeight="1"/>
+    <row r="132" ht="16.5" customHeight="1"/>
+    <row r="133" ht="16.5" customHeight="1"/>
+    <row r="134" ht="16.5" customHeight="1"/>
+    <row r="135" ht="16.5" customHeight="1"/>
+    <row r="136" ht="16.5" customHeight="1"/>
+    <row r="137" ht="16.5" customHeight="1"/>
+    <row r="138" ht="16.5" customHeight="1"/>
+    <row r="139" ht="16.5" customHeight="1"/>
+    <row r="140" ht="16.5" customHeight="1"/>
+    <row r="141" ht="16.5" customHeight="1"/>
+    <row r="142" ht="16.5" customHeight="1"/>
+    <row r="143" ht="16.5" customHeight="1"/>
+    <row r="144" ht="16.5" customHeight="1"/>
+    <row r="145" ht="16.5" customHeight="1"/>
+    <row r="146" ht="16.5" customHeight="1"/>
+    <row r="147" ht="16.5" customHeight="1"/>
+    <row r="148" ht="16.5" customHeight="1"/>
+    <row r="149" ht="16.5" customHeight="1"/>
+    <row r="150" ht="16.5" customHeight="1"/>
+    <row r="151" ht="16.5" customHeight="1"/>
+    <row r="152" ht="16.5" customHeight="1"/>
+    <row r="153" ht="16.5" customHeight="1"/>
+    <row r="154" ht="16.5" customHeight="1"/>
+    <row r="155" ht="16.5" customHeight="1"/>
+    <row r="156" ht="16.5" customHeight="1"/>
+    <row r="157" ht="16.5" customHeight="1"/>
+    <row r="158" ht="16.5" customHeight="1"/>
+    <row r="159" ht="16.5" customHeight="1"/>
+    <row r="160" ht="16.5" customHeight="1"/>
+    <row r="161" ht="16.5" customHeight="1"/>
+    <row r="162" ht="16.5" customHeight="1"/>
+    <row r="163" ht="16.5" customHeight="1"/>
+    <row r="164" ht="16.5" customHeight="1"/>
+    <row r="165" ht="16.5" customHeight="1"/>
+    <row r="166" ht="16.5" customHeight="1"/>
+    <row r="167" ht="16.5" customHeight="1"/>
+    <row r="168" ht="16.5" customHeight="1"/>
+    <row r="169" ht="16.5" customHeight="1"/>
+    <row r="170" ht="16.5" customHeight="1"/>
+    <row r="171" ht="16.5" customHeight="1"/>
+    <row r="172" ht="16.5" customHeight="1"/>
+    <row r="173" ht="16.5" customHeight="1"/>
+    <row r="174" ht="16.5" customHeight="1"/>
+    <row r="175" ht="16.5" customHeight="1"/>
+    <row r="176" ht="16.5" customHeight="1"/>
+    <row r="177" ht="16.5" customHeight="1"/>
+    <row r="178" ht="16.5" customHeight="1"/>
+    <row r="179" ht="16.5" customHeight="1"/>
+    <row r="180" ht="16.5" customHeight="1"/>
+    <row r="181" ht="16.5" customHeight="1"/>
+    <row r="182" ht="16.5" customHeight="1"/>
+    <row r="183" ht="16.5" customHeight="1"/>
+    <row r="184" ht="16.5" customHeight="1"/>
+    <row r="185" ht="16.5" customHeight="1"/>
+    <row r="186" ht="16.5" customHeight="1"/>
+    <row r="187" ht="16.5" customHeight="1"/>
+    <row r="188" ht="16.5" customHeight="1"/>
+    <row r="189" ht="16.5" customHeight="1"/>
+    <row r="190" ht="16.5" customHeight="1"/>
+    <row r="191" ht="16.5" customHeight="1"/>
+    <row r="192" ht="16.5" customHeight="1"/>
+    <row r="193" ht="16.5" customHeight="1"/>
+    <row r="194" ht="16.5" customHeight="1"/>
+    <row r="195" ht="16.5" customHeight="1"/>
+    <row r="196" ht="16.5" customHeight="1"/>
+    <row r="197" ht="16.5" customHeight="1"/>
+    <row r="198" ht="16.5" customHeight="1"/>
+    <row r="199" ht="16.5" customHeight="1"/>
+    <row r="200" ht="16.5" customHeight="1"/>
+    <row r="201" ht="16.5" customHeight="1"/>
+    <row r="202" ht="16.5" customHeight="1"/>
+    <row r="203" ht="16.5" customHeight="1"/>
+    <row r="204" ht="16.5" customHeight="1"/>
+    <row r="205" ht="16.5" customHeight="1"/>
+    <row r="206" ht="16.5" customHeight="1"/>
+    <row r="207" ht="16.5" customHeight="1"/>
+    <row r="208" ht="16.5" customHeight="1"/>
+    <row r="209" ht="16.5" customHeight="1"/>
+    <row r="210" ht="16.5" customHeight="1"/>
+    <row r="211" ht="16.5" customHeight="1"/>
+    <row r="212" ht="16.5" customHeight="1"/>
+    <row r="213" ht="16.5" customHeight="1"/>
+    <row r="214" ht="16.5" customHeight="1"/>
+    <row r="215" ht="16.5" customHeight="1"/>
+    <row r="216" ht="16.5" customHeight="1"/>
+    <row r="217" ht="16.5" customHeight="1"/>
+    <row r="218" ht="16.5" customHeight="1"/>
+    <row r="219" ht="16.5" customHeight="1"/>
+    <row r="220" ht="16.5" customHeight="1"/>
+    <row r="221" ht="16.5" customHeight="1"/>
+    <row r="222" ht="16.5" customHeight="1"/>
+    <row r="223" ht="16.5" customHeight="1"/>
+    <row r="224" ht="16.5" customHeight="1"/>
+    <row r="225" ht="16.5" customHeight="1"/>
+    <row r="226" ht="16.5" customHeight="1"/>
+    <row r="227" ht="16.5" customHeight="1"/>
+    <row r="228" ht="16.5" customHeight="1"/>
+    <row r="229" ht="16.5" customHeight="1"/>
+    <row r="230" ht="16.5" customHeight="1"/>
+    <row r="231" ht="16.5" customHeight="1"/>
+    <row r="232" ht="16.5" customHeight="1"/>
+    <row r="233" ht="16.5" customHeight="1"/>
+    <row r="234" ht="16.5" customHeight="1"/>
+    <row r="235" ht="16.5" customHeight="1"/>
+    <row r="236" ht="16.5" customHeight="1"/>
+    <row r="237" ht="16.5" customHeight="1"/>
+    <row r="238" ht="16.5" customHeight="1"/>
+    <row r="239" ht="16.5" customHeight="1"/>
+    <row r="240" ht="16.5" customHeight="1"/>
+    <row r="241" ht="16.5" customHeight="1"/>
+    <row r="242" ht="16.5" customHeight="1"/>
+    <row r="243" ht="16.5" customHeight="1"/>
+    <row r="244" ht="16.5" customHeight="1"/>
+    <row r="245" ht="16.5" customHeight="1"/>
+    <row r="246" ht="16.5" customHeight="1"/>
+    <row r="247" ht="16.5" customHeight="1"/>
+    <row r="248" ht="16.5" customHeight="1"/>
+    <row r="249" ht="16.5" customHeight="1"/>
+    <row r="250" ht="16.5" customHeight="1"/>
+    <row r="251" ht="16.5" customHeight="1"/>
+    <row r="252" ht="16.5" customHeight="1"/>
+    <row r="253" ht="16.5" customHeight="1"/>
+    <row r="254" ht="16.5" customHeight="1"/>
+    <row r="255" ht="16.5" customHeight="1"/>
+    <row r="256" ht="16.5" customHeight="1"/>
+    <row r="257" ht="16.5" customHeight="1"/>
+    <row r="258" ht="16.5" customHeight="1"/>
+    <row r="259" ht="16.5" customHeight="1"/>
+    <row r="260" ht="16.5" customHeight="1"/>
+    <row r="261" ht="16.5" customHeight="1"/>
+    <row r="262" ht="16.5" customHeight="1"/>
+    <row r="263" ht="16.5" customHeight="1"/>
+    <row r="264" ht="16.5" customHeight="1"/>
+    <row r="265" ht="16.5" customHeight="1"/>
+    <row r="266" ht="16.5" customHeight="1"/>
+    <row r="267" ht="16.5" customHeight="1"/>
+    <row r="268" ht="16.5" customHeight="1"/>
+    <row r="269" ht="16.5" customHeight="1"/>
+    <row r="270" ht="16.5" customHeight="1"/>
+    <row r="271" ht="16.5" customHeight="1"/>
+    <row r="272" ht="16.5" customHeight="1"/>
+    <row r="273" ht="16.5" customHeight="1"/>
+    <row r="274" ht="16.5" customHeight="1"/>
+    <row r="275" ht="16.5" customHeight="1"/>
+    <row r="276" ht="16.5" customHeight="1"/>
+    <row r="277" ht="16.5" customHeight="1"/>
+    <row r="278" ht="16.5" customHeight="1"/>
+    <row r="279" ht="16.5" customHeight="1"/>
+    <row r="280" ht="16.5" customHeight="1"/>
+    <row r="281" ht="16.5" customHeight="1"/>
+    <row r="282" ht="16.5" customHeight="1"/>
+    <row r="283" ht="16.5" customHeight="1"/>
+    <row r="284" ht="16.5" customHeight="1"/>
+    <row r="285" ht="16.5" customHeight="1"/>
+    <row r="286" ht="16.5" customHeight="1"/>
+    <row r="287" ht="16.5" customHeight="1"/>
+    <row r="288" ht="16.5" customHeight="1"/>
+    <row r="289" ht="16.5" customHeight="1"/>
+    <row r="290" ht="16.5" customHeight="1"/>
+    <row r="291" ht="16.5" customHeight="1"/>
+    <row r="292" ht="16.5" customHeight="1"/>
+    <row r="293" ht="16.5" customHeight="1"/>
+    <row r="294" ht="16.5" customHeight="1"/>
+    <row r="295" ht="16.5" customHeight="1"/>
+    <row r="296" ht="16.5" customHeight="1"/>
+    <row r="297" ht="16.5" customHeight="1"/>
+    <row r="298" ht="16.5" customHeight="1"/>
+    <row r="299" ht="16.5" customHeight="1"/>
+    <row r="300" ht="16.5" customHeight="1"/>
+    <row r="301" ht="16.5" customHeight="1"/>
+    <row r="302" ht="16.5" customHeight="1"/>
+    <row r="303" ht="16.5" customHeight="1"/>
+    <row r="304" ht="16.5" customHeight="1"/>
+    <row r="305" ht="16.5" customHeight="1"/>
+    <row r="306" ht="16.5" customHeight="1"/>
+    <row r="307" ht="16.5" customHeight="1"/>
+    <row r="308" ht="16.5" customHeight="1"/>
+    <row r="309" ht="16.5" customHeight="1"/>
+    <row r="310" ht="16.5" customHeight="1"/>
+    <row r="311" ht="16.5" customHeight="1"/>
+    <row r="312" ht="16.5" customHeight="1"/>
+    <row r="313" ht="16.5" customHeight="1"/>
+    <row r="314" ht="16.5" customHeight="1"/>
+    <row r="315" ht="16.5" customHeight="1"/>
+    <row r="316" ht="16.5" customHeight="1"/>
+    <row r="317" ht="16.5" customHeight="1"/>
+    <row r="318" ht="16.5" customHeight="1"/>
+    <row r="319" ht="16.5" customHeight="1"/>
+    <row r="320" ht="16.5" customHeight="1"/>
+    <row r="321" ht="16.5" customHeight="1"/>
+    <row r="322" ht="16.5" customHeight="1"/>
+    <row r="323" ht="16.5" customHeight="1"/>
+    <row r="324" ht="16.5" customHeight="1"/>
+    <row r="325" ht="16.5" customHeight="1"/>
+    <row r="326" ht="16.5" customHeight="1"/>
+    <row r="327" ht="16.5" customHeight="1"/>
+    <row r="328" ht="16.5" customHeight="1"/>
+    <row r="329" ht="16.5" customHeight="1"/>
+    <row r="330" ht="16.5" customHeight="1"/>
+    <row r="331" ht="16.5" customHeight="1"/>
+    <row r="332" ht="16.5" customHeight="1"/>
+    <row r="333" ht="16.5" customHeight="1"/>
+    <row r="334" ht="16.5" customHeight="1"/>
+    <row r="335" ht="16.5" customHeight="1"/>
+    <row r="336" ht="16.5" customHeight="1"/>
+    <row r="337" ht="16.5" customHeight="1"/>
+    <row r="338" ht="16.5" customHeight="1"/>
+    <row r="339" ht="16.5" customHeight="1"/>
+    <row r="340" ht="16.5" customHeight="1"/>
+    <row r="341" ht="16.5" customHeight="1"/>
+    <row r="342" ht="16.5" customHeight="1"/>
+    <row r="343" ht="16.5" customHeight="1"/>
+    <row r="344" ht="16.5" customHeight="1"/>
+    <row r="345" ht="16.5" customHeight="1"/>
+    <row r="346" ht="16.5" customHeight="1"/>
+    <row r="347" ht="16.5" customHeight="1"/>
+    <row r="348" ht="16.5" customHeight="1"/>
+    <row r="349" ht="16.5" customHeight="1"/>
+    <row r="350" ht="16.5" customHeight="1"/>
+    <row r="351" ht="16.5" customHeight="1"/>
+    <row r="352" ht="16.5" customHeight="1"/>
+    <row r="353" ht="16.5" customHeight="1"/>
+    <row r="354" ht="16.5" customHeight="1"/>
+    <row r="355" ht="16.5" customHeight="1"/>
+    <row r="356" ht="16.5" customHeight="1"/>
+    <row r="357" ht="16.5" customHeight="1"/>
+    <row r="358" ht="16.5" customHeight="1"/>
+    <row r="359" ht="16.5" customHeight="1"/>
+    <row r="360" ht="16.5" customHeight="1"/>
+    <row r="361" ht="16.5" customHeight="1"/>
+    <row r="362" ht="16.5" customHeight="1"/>
+    <row r="363" ht="16.5" customHeight="1"/>
+    <row r="364" ht="16.5" customHeight="1"/>
+    <row r="365" ht="16.5" customHeight="1"/>
+    <row r="366" ht="16.5" customHeight="1"/>
+    <row r="367" ht="16.5" customHeight="1"/>
+    <row r="368" ht="16.5" customHeight="1"/>
+    <row r="369" ht="16.5" customHeight="1"/>
+    <row r="370" ht="16.5" customHeight="1"/>
+    <row r="371" ht="16.5" customHeight="1"/>
+    <row r="372" ht="16.5" customHeight="1"/>
+    <row r="373" ht="16.5" customHeight="1"/>
+    <row r="374" ht="16.5" customHeight="1"/>
+    <row r="375" ht="16.5" customHeight="1"/>
+    <row r="376" ht="16.5" customHeight="1"/>
+    <row r="377" ht="16.5" customHeight="1"/>
+    <row r="378" ht="16.5" customHeight="1"/>
+    <row r="379" ht="16.5" customHeight="1"/>
+    <row r="380" ht="16.5" customHeight="1"/>
+    <row r="381" ht="16.5" customHeight="1"/>
+    <row r="382" ht="16.5" customHeight="1"/>
+    <row r="383" ht="16.5" customHeight="1"/>
+    <row r="384" ht="16.5" customHeight="1"/>
+    <row r="385" ht="16.5" customHeight="1"/>
+    <row r="386" ht="16.5" customHeight="1"/>
+    <row r="387" ht="16.5" customHeight="1"/>
+    <row r="388" ht="16.5" customHeight="1"/>
+    <row r="389" ht="16.5" customHeight="1"/>
+    <row r="390" ht="16.5" customHeight="1"/>
+    <row r="391" ht="16.5" customHeight="1"/>
+    <row r="392" ht="16.5" customHeight="1"/>
+    <row r="393" ht="16.5" customHeight="1"/>
+    <row r="394" ht="16.5" customHeight="1"/>
+    <row r="395" ht="16.5" customHeight="1"/>
+    <row r="396" ht="16.5" customHeight="1"/>
+    <row r="397" ht="16.5" customHeight="1"/>
+    <row r="398" ht="16.5" customHeight="1"/>
+    <row r="399" ht="16.5" customHeight="1"/>
+    <row r="400" ht="16.5" customHeight="1"/>
+    <row r="401" ht="16.5" customHeight="1"/>
+    <row r="402" ht="16.5" customHeight="1"/>
+    <row r="403" ht="16.5" customHeight="1"/>
+    <row r="404" ht="16.5" customHeight="1"/>
+    <row r="405" ht="16.5" customHeight="1"/>
+    <row r="406" ht="16.5" customHeight="1"/>
+    <row r="407" ht="16.5" customHeight="1"/>
+    <row r="408" ht="16.5" customHeight="1"/>
+    <row r="409" ht="16.5" customHeight="1"/>
+    <row r="410" ht="16.5" customHeight="1"/>
+    <row r="411" ht="16.5" customHeight="1"/>
+    <row r="412" ht="16.5" customHeight="1"/>
+    <row r="413" ht="16.5" customHeight="1"/>
+    <row r="414" ht="16.5" customHeight="1"/>
+    <row r="415" ht="16.5" customHeight="1"/>
+    <row r="416" ht="16.5" customHeight="1"/>
+    <row r="417" ht="16.5" customHeight="1"/>
+    <row r="418" ht="16.5" customHeight="1"/>
+    <row r="419" ht="16.5" customHeight="1"/>
+    <row r="420" ht="16.5" customHeight="1"/>
+    <row r="421" ht="16.5" customHeight="1"/>
+    <row r="422" ht="16.5" customHeight="1"/>
+    <row r="423" ht="16.5" customHeight="1"/>
+    <row r="424" ht="16.5" customHeight="1"/>
+    <row r="425" ht="16.5" customHeight="1"/>
+    <row r="426" ht="16.5" customHeight="1"/>
+    <row r="427" ht="16.5" customHeight="1"/>
+    <row r="428" ht="16.5" customHeight="1"/>
+    <row r="429" ht="16.5" customHeight="1"/>
+    <row r="430" ht="16.5" customHeight="1"/>
+    <row r="431" ht="16.5" customHeight="1"/>
+    <row r="432" ht="16.5" customHeight="1"/>
+    <row r="433" ht="16.5" customHeight="1"/>
+    <row r="434" ht="16.5" customHeight="1"/>
+    <row r="435" ht="16.5" customHeight="1"/>
+    <row r="436" ht="16.5" customHeight="1"/>
+    <row r="437" ht="16.5" customHeight="1"/>
+    <row r="438" ht="16.5" customHeight="1"/>
+    <row r="439" ht="16.5" customHeight="1"/>
+    <row r="440" ht="16.5" customHeight="1"/>
+    <row r="441" ht="16.5" customHeight="1"/>
+    <row r="442" ht="16.5" customHeight="1"/>
+    <row r="443" ht="16.5" customHeight="1"/>
+    <row r="444" ht="16.5" customHeight="1"/>
+    <row r="445" ht="16.5" customHeight="1"/>
+    <row r="446" ht="16.5" customHeight="1"/>
+    <row r="447" ht="16.5" customHeight="1"/>
+    <row r="448" ht="16.5" customHeight="1"/>
+    <row r="449" ht="16.5" customHeight="1"/>
+    <row r="450" ht="16.5" customHeight="1"/>
+    <row r="451" ht="16.5" customHeight="1"/>
+    <row r="452" ht="16.5" customHeight="1"/>
+    <row r="453" ht="16.5" customHeight="1"/>
+    <row r="454" ht="16.5" customHeight="1"/>
+    <row r="455" ht="16.5" customHeight="1"/>
+    <row r="456" ht="16.5" customHeight="1"/>
+    <row r="457" ht="16.5" customHeight="1"/>
+    <row r="458" ht="16.5" customHeight="1"/>
+    <row r="459" ht="16.5" customHeight="1"/>
+    <row r="460" ht="16.5" customHeight="1"/>
+    <row r="461" ht="16.5" customHeight="1"/>
+    <row r="462" ht="16.5" customHeight="1"/>
+    <row r="463" ht="16.5" customHeight="1"/>
+    <row r="464" ht="16.5" customHeight="1"/>
+    <row r="465" ht="16.5" customHeight="1"/>
+    <row r="466" ht="16.5" customHeight="1"/>
+    <row r="467" ht="16.5" customHeight="1"/>
+    <row r="468" ht="16.5" customHeight="1"/>
+    <row r="469" ht="16.5" customHeight="1"/>
+    <row r="470" ht="16.5" customHeight="1"/>
+    <row r="471" ht="16.5" customHeight="1"/>
+    <row r="472" ht="16.5" customHeight="1"/>
+    <row r="473" ht="16.5" customHeight="1"/>
+    <row r="474" ht="16.5" customHeight="1"/>
+    <row r="475" ht="16.5" customHeight="1"/>
+    <row r="476" ht="16.5" customHeight="1"/>
+    <row r="477" ht="16.5" customHeight="1"/>
+    <row r="478" ht="16.5" customHeight="1"/>
+    <row r="479" ht="16.5" customHeight="1"/>
+    <row r="480" ht="16.5" customHeight="1"/>
+    <row r="481" ht="16.5" customHeight="1"/>
+    <row r="482" ht="16.5" customHeight="1"/>
+    <row r="483" ht="16.5" customHeight="1"/>
+    <row r="484" ht="16.5" customHeight="1"/>
+    <row r="485" ht="16.5" customHeight="1"/>
+    <row r="486" ht="16.5" customHeight="1"/>
+    <row r="487" ht="16.5" customHeight="1"/>
+    <row r="488" ht="16.5" customHeight="1"/>
+    <row r="489" ht="16.5" customHeight="1"/>
+    <row r="490" ht="16.5" customHeight="1"/>
+    <row r="491" ht="16.5" customHeight="1"/>
+    <row r="492" ht="16.5" customHeight="1"/>
+    <row r="493" ht="16.5" customHeight="1"/>
+    <row r="494" ht="16.5" customHeight="1"/>
+    <row r="495" ht="16.5" customHeight="1"/>
+    <row r="496" ht="16.5" customHeight="1"/>
+    <row r="497" ht="16.5" customHeight="1"/>
+    <row r="498" ht="16.5" customHeight="1"/>
+    <row r="499" ht="16.5" customHeight="1"/>
+    <row r="500" ht="16.5" customHeight="1"/>
+    <row r="501" ht="16.5" customHeight="1"/>
+    <row r="502" ht="16.5" customHeight="1"/>
+    <row r="503" ht="16.5" customHeight="1"/>
+    <row r="504" ht="16.5" customHeight="1"/>
+    <row r="505" ht="16.5" customHeight="1"/>
+    <row r="506" ht="16.5" customHeight="1"/>
+    <row r="507" ht="16.5" customHeight="1"/>
+    <row r="508" ht="16.5" customHeight="1"/>
+    <row r="509" ht="16.5" customHeight="1"/>
+    <row r="510" ht="16.5" customHeight="1"/>
+    <row r="511" ht="16.5" customHeight="1"/>
+    <row r="512" ht="16.5" customHeight="1"/>
+    <row r="513" ht="16.5" customHeight="1"/>
+    <row r="514" ht="16.5" customHeight="1"/>
+    <row r="515" ht="16.5" customHeight="1"/>
+    <row r="516" ht="16.5" customHeight="1"/>
+    <row r="517" ht="16.5" customHeight="1"/>
+    <row r="518" ht="16.5" customHeight="1"/>
+    <row r="519" ht="16.5" customHeight="1"/>
+    <row r="520" ht="16.5" customHeight="1"/>
+    <row r="521" ht="16.5" customHeight="1"/>
+    <row r="522" ht="16.5" customHeight="1"/>
+    <row r="523" ht="16.5" customHeight="1"/>
+    <row r="524" ht="16.5" customHeight="1"/>
+    <row r="525" ht="16.5" customHeight="1"/>
+    <row r="526" ht="16.5" customHeight="1"/>
+    <row r="527" ht="16.5" customHeight="1"/>
+    <row r="528" ht="16.5" customHeight="1"/>
+    <row r="529" ht="16.5" customHeight="1"/>
+    <row r="530" ht="16.5" customHeight="1"/>
+    <row r="531" ht="16.5" customHeight="1"/>
+    <row r="532" ht="16.5" customHeight="1"/>
+    <row r="533" ht="16.5" customHeight="1"/>
+    <row r="534" ht="16.5" customHeight="1"/>
+    <row r="535" ht="16.5" customHeight="1"/>
+    <row r="536" ht="16.5" customHeight="1"/>
+    <row r="537" ht="16.5" customHeight="1"/>
+    <row r="538" ht="16.5" customHeight="1"/>
+    <row r="539" ht="16.5" customHeight="1"/>
+    <row r="540" ht="16.5" customHeight="1"/>
+    <row r="541" ht="16.5" customHeight="1"/>
+    <row r="542" ht="16.5" customHeight="1"/>
+    <row r="543" ht="16.5" customHeight="1"/>
+    <row r="544" ht="16.5" customHeight="1"/>
+    <row r="545" ht="16.5" customHeight="1"/>
+    <row r="546" ht="16.5" customHeight="1"/>
+    <row r="547" ht="16.5" customHeight="1"/>
+    <row r="548" ht="16.5" customHeight="1"/>
+    <row r="549" ht="16.5" customHeight="1"/>
+    <row r="550" ht="16.5" customHeight="1"/>
+    <row r="551" ht="16.5" customHeight="1"/>
+    <row r="552" ht="16.5" customHeight="1"/>
+    <row r="553" ht="16.5" customHeight="1"/>
+    <row r="554" ht="16.5" customHeight="1"/>
+    <row r="555" ht="16.5" customHeight="1"/>
+    <row r="556" ht="16.5" customHeight="1"/>
+    <row r="557" ht="16.5" customHeight="1"/>
+    <row r="558" ht="16.5" customHeight="1"/>
+    <row r="559" ht="16.5" customHeight="1"/>
+    <row r="560" ht="16.5" customHeight="1"/>
+    <row r="561" ht="16.5" customHeight="1"/>
+    <row r="562" ht="16.5" customHeight="1"/>
+    <row r="563" ht="16.5" customHeight="1"/>
+    <row r="564" ht="16.5" customHeight="1"/>
+    <row r="565" ht="16.5" customHeight="1"/>
+    <row r="566" ht="16.5" customHeight="1"/>
+    <row r="567" ht="16.5" customHeight="1"/>
+    <row r="568" ht="16.5" customHeight="1"/>
+    <row r="569" ht="16.5" customHeight="1"/>
+    <row r="570" ht="16.5" customHeight="1"/>
+    <row r="571" ht="16.5" customHeight="1"/>
+    <row r="572" ht="16.5" customHeight="1"/>
+    <row r="573" ht="16.5" customHeight="1"/>
+    <row r="574" ht="16.5" customHeight="1"/>
+    <row r="575" ht="16.5" customHeight="1"/>
+    <row r="576" ht="16.5" customHeight="1"/>
+    <row r="577" ht="16.5" customHeight="1"/>
+    <row r="578" ht="16.5" customHeight="1"/>
+    <row r="579" ht="16.5" customHeight="1"/>
+    <row r="580" ht="16.5" customHeight="1"/>
+    <row r="581" ht="16.5" customHeight="1"/>
+    <row r="582" ht="16.5" customHeight="1"/>
+    <row r="583" ht="16.5" customHeight="1"/>
+    <row r="584" ht="16.5" customHeight="1"/>
+    <row r="585" ht="16.5" customHeight="1"/>
+    <row r="586" ht="16.5" customHeight="1"/>
+    <row r="587" ht="16.5" customHeight="1"/>
+    <row r="588" ht="16.5" customHeight="1"/>
+    <row r="589" ht="16.5" customHeight="1"/>
+    <row r="590" ht="16.5" customHeight="1"/>
+    <row r="591" ht="16.5" customHeight="1"/>
+    <row r="592" ht="16.5" customHeight="1"/>
+    <row r="593" ht="16.5" customHeight="1"/>
+    <row r="594" ht="16.5" customHeight="1"/>
+    <row r="595" ht="16.5" customHeight="1"/>
+    <row r="596" ht="16.5" customHeight="1"/>
+    <row r="597" ht="16.5" customHeight="1"/>
+    <row r="598" ht="16.5" customHeight="1"/>
+    <row r="599" ht="16.5" customHeight="1"/>
+    <row r="600" ht="16.5" customHeight="1"/>
+    <row r="601" ht="16.5" customHeight="1"/>
+    <row r="602" ht="16.5" customHeight="1"/>
+    <row r="603" ht="16.5" customHeight="1"/>
+    <row r="604" ht="16.5" customHeight="1"/>
+    <row r="605" ht="16.5" customHeight="1"/>
+    <row r="606" ht="16.5" customHeight="1"/>
+    <row r="607" ht="16.5" customHeight="1"/>
+    <row r="608" ht="16.5" customHeight="1"/>
+    <row r="609" ht="16.5" customHeight="1"/>
+    <row r="610" ht="16.5" customHeight="1"/>
+    <row r="611" ht="16.5" customHeight="1"/>
+    <row r="612" ht="16.5" customHeight="1"/>
+    <row r="613" ht="16.5" customHeight="1"/>
+    <row r="614" ht="16.5" customHeight="1"/>
+    <row r="615" ht="16.5" customHeight="1"/>
+    <row r="616" ht="16.5" customHeight="1"/>
+    <row r="617" ht="16.5" customHeight="1"/>
+    <row r="618" ht="16.5" customHeight="1"/>
+    <row r="619" ht="16.5" customHeight="1"/>
+    <row r="620" ht="16.5" customHeight="1"/>
+    <row r="621" ht="16.5" customHeight="1"/>
+    <row r="622" ht="16.5" customHeight="1"/>
+    <row r="623" ht="16.5" customHeight="1"/>
+    <row r="624" ht="16.5" customHeight="1"/>
+    <row r="625" ht="16.5" customHeight="1"/>
+    <row r="626" ht="16.5" customHeight="1"/>
+    <row r="627" ht="16.5" customHeight="1"/>
+    <row r="628" ht="16.5" customHeight="1"/>
+    <row r="629" ht="16.5" customHeight="1"/>
+    <row r="630" ht="16.5" customHeight="1"/>
+    <row r="631" ht="16.5" customHeight="1"/>
+    <row r="632" ht="16.5" customHeight="1"/>
+    <row r="633" ht="16.5" customHeight="1"/>
+    <row r="634" ht="16.5" customHeight="1"/>
+    <row r="635" ht="16.5" customHeight="1"/>
+    <row r="636" ht="16.5" customHeight="1"/>
+    <row r="637" ht="16.5" customHeight="1"/>
+    <row r="638" ht="16.5" customHeight="1"/>
+    <row r="639" ht="16.5" customHeight="1"/>
+    <row r="640" ht="16.5" customHeight="1"/>
+    <row r="641" ht="16.5" customHeight="1"/>
+    <row r="642" ht="16.5" customHeight="1"/>
+    <row r="643" ht="16.5" customHeight="1"/>
+    <row r="644" ht="16.5" customHeight="1"/>
+    <row r="645" ht="16.5" customHeight="1"/>
+    <row r="646" ht="16.5" customHeight="1"/>
+    <row r="647" ht="16.5" customHeight="1"/>
+    <row r="648" ht="16.5" customHeight="1"/>
+    <row r="649" ht="16.5" customHeight="1"/>
+    <row r="650" ht="16.5" customHeight="1"/>
+    <row r="651" ht="16.5" customHeight="1"/>
+    <row r="652" ht="16.5" customHeight="1"/>
+    <row r="653" ht="16.5" customHeight="1"/>
+    <row r="654" ht="16.5" customHeight="1"/>
+    <row r="655" ht="16.5" customHeight="1"/>
+    <row r="656" ht="16.5" customHeight="1"/>
+    <row r="657" ht="16.5" customHeight="1"/>
+    <row r="658" ht="16.5" customHeight="1"/>
+    <row r="659" ht="16.5" customHeight="1"/>
+    <row r="660" ht="16.5" customHeight="1"/>
+    <row r="661" ht="16.5" customHeight="1"/>
+    <row r="662" ht="16.5" customHeight="1"/>
+    <row r="663" ht="16.5" customHeight="1"/>
+    <row r="664" ht="16.5" customHeight="1"/>
+    <row r="665" ht="16.5" customHeight="1"/>
+    <row r="666" ht="16.5" customHeight="1"/>
+    <row r="667" ht="16.5" customHeight="1"/>
+    <row r="668" ht="16.5" customHeight="1"/>
+    <row r="669" ht="16.5" customHeight="1"/>
+    <row r="670" ht="16.5" customHeight="1"/>
+    <row r="671" ht="16.5" customHeight="1"/>
+    <row r="672" ht="16.5" customHeight="1"/>
+    <row r="673" ht="16.5" customHeight="1"/>
+    <row r="674" ht="16.5" customHeight="1"/>
+    <row r="675" ht="16.5" customHeight="1"/>
+    <row r="676" ht="16.5" customHeight="1"/>
+    <row r="677" ht="16.5" customHeight="1"/>
+    <row r="678" ht="16.5" customHeight="1"/>
+    <row r="679" ht="16.5" customHeight="1"/>
+    <row r="680" ht="16.5" customHeight="1"/>
+    <row r="681" ht="16.5" customHeight="1"/>
+    <row r="682" ht="16.5" customHeight="1"/>
+    <row r="683" ht="16.5" customHeight="1"/>
+    <row r="684" ht="16.5" customHeight="1"/>
+    <row r="685" ht="16.5" customHeight="1"/>
+    <row r="686" ht="16.5" customHeight="1"/>
+    <row r="687" ht="16.5" customHeight="1"/>
+    <row r="688" ht="16.5" customHeight="1"/>
+    <row r="689" ht="16.5" customHeight="1"/>
+    <row r="690" ht="16.5" customHeight="1"/>
+    <row r="691" ht="16.5" customHeight="1"/>
+    <row r="692" ht="16.5" customHeight="1"/>
+    <row r="693" ht="16.5" customHeight="1"/>
+    <row r="694" ht="16.5" customHeight="1"/>
+    <row r="695" ht="16.5" customHeight="1"/>
+    <row r="696" ht="16.5" customHeight="1"/>
+    <row r="697" ht="16.5" customHeight="1"/>
+    <row r="698" ht="16.5" customHeight="1"/>
+    <row r="699" ht="16.5" customHeight="1"/>
+    <row r="700" ht="16.5" customHeight="1"/>
+    <row r="701" ht="16.5" customHeight="1"/>
+    <row r="702" ht="16.5" customHeight="1"/>
+    <row r="703" ht="16.5" customHeight="1"/>
+    <row r="704" ht="16.5" customHeight="1"/>
+    <row r="705" ht="16.5" customHeight="1"/>
+    <row r="706" ht="16.5" customHeight="1"/>
+    <row r="707" ht="16.5" customHeight="1"/>
+    <row r="708" ht="16.5" customHeight="1"/>
+    <row r="709" ht="16.5" customHeight="1"/>
+    <row r="710" ht="16.5" customHeight="1"/>
+    <row r="711" ht="16.5" customHeight="1"/>
+    <row r="712" ht="16.5" customHeight="1"/>
+    <row r="713" ht="16.5" customHeight="1"/>
+    <row r="714" ht="16.5" customHeight="1"/>
+    <row r="715" ht="16.5" customHeight="1"/>
+    <row r="716" ht="16.5" customHeight="1"/>
+    <row r="717" ht="16.5" customHeight="1"/>
+    <row r="718" ht="16.5" customHeight="1"/>
+    <row r="719" ht="16.5" customHeight="1"/>
+    <row r="720" ht="16.5" customHeight="1"/>
+    <row r="721" ht="16.5" customHeight="1"/>
+    <row r="722" ht="16.5" customHeight="1"/>
+    <row r="723" ht="16.5" customHeight="1"/>
+    <row r="724" ht="16.5" customHeight="1"/>
+    <row r="725" ht="16.5" customHeight="1"/>
+    <row r="726" ht="16.5" customHeight="1"/>
+    <row r="727" ht="16.5" customHeight="1"/>
+    <row r="728" ht="16.5" customHeight="1"/>
+    <row r="729" ht="16.5" customHeight="1"/>
+    <row r="730" ht="16.5" customHeight="1"/>
+    <row r="731" ht="16.5" customHeight="1"/>
+    <row r="732" ht="16.5" customHeight="1"/>
+    <row r="733" ht="16.5" customHeight="1"/>
+    <row r="734" ht="16.5" customHeight="1"/>
+    <row r="735" ht="16.5" customHeight="1"/>
+    <row r="736" ht="16.5" customHeight="1"/>
+    <row r="737" ht="16.5" customHeight="1"/>
+    <row r="738" ht="16.5" customHeight="1"/>
+    <row r="739" ht="16.5" customHeight="1"/>
+    <row r="740" ht="16.5" customHeight="1"/>
+    <row r="741" ht="16.5" customHeight="1"/>
+    <row r="742" ht="16.5" customHeight="1"/>
+    <row r="743" ht="16.5" customHeight="1"/>
+    <row r="744" ht="16.5" customHeight="1"/>
+    <row r="745" ht="16.5" customHeight="1"/>
+    <row r="746" ht="16.5" customHeight="1"/>
+    <row r="747" ht="16.5" customHeight="1"/>
+    <row r="748" ht="16.5" customHeight="1"/>
+    <row r="749" ht="16.5" customHeight="1"/>
+    <row r="750" ht="16.5" customHeight="1"/>
+    <row r="751" ht="16.5" customHeight="1"/>
+    <row r="752" ht="16.5" customHeight="1"/>
+    <row r="753" ht="16.5" customHeight="1"/>
+    <row r="754" ht="16.5" customHeight="1"/>
+    <row r="755" ht="16.5" customHeight="1"/>
+    <row r="756" ht="16.5" customHeight="1"/>
+    <row r="757" ht="16.5" customHeight="1"/>
+    <row r="758" ht="16.5" customHeight="1"/>
+    <row r="759" ht="16.5" customHeight="1"/>
+    <row r="760" ht="16.5" customHeight="1"/>
+    <row r="761" ht="16.5" customHeight="1"/>
+    <row r="762" ht="16.5" customHeight="1"/>
+    <row r="763" ht="16.5" customHeight="1"/>
+    <row r="764" ht="16.5" customHeight="1"/>
+    <row r="765" ht="16.5" customHeight="1"/>
+    <row r="766" ht="16.5" customHeight="1"/>
+    <row r="767" ht="16.5" customHeight="1"/>
+    <row r="768" ht="16.5" customHeight="1"/>
+    <row r="769" ht="16.5" customHeight="1"/>
+    <row r="770" ht="16.5" customHeight="1"/>
+    <row r="771" ht="16.5" customHeight="1"/>
+    <row r="772" ht="16.5" customHeight="1"/>
+    <row r="773" ht="16.5" customHeight="1"/>
+    <row r="774" ht="16.5" customHeight="1"/>
+    <row r="775" ht="16.5" customHeight="1"/>
+    <row r="776" ht="16.5" customHeight="1"/>
+    <row r="777" ht="16.5" customHeight="1"/>
+    <row r="778" ht="16.5" customHeight="1"/>
+    <row r="779" ht="16.5" customHeight="1"/>
+    <row r="780" ht="16.5" customHeight="1"/>
+    <row r="781" ht="16.5" customHeight="1"/>
+    <row r="782" ht="16.5" customHeight="1"/>
+    <row r="783" ht="16.5" customHeight="1"/>
+    <row r="784" ht="16.5" customHeight="1"/>
+    <row r="785" ht="16.5" customHeight="1"/>
+    <row r="786" ht="16.5" customHeight="1"/>
+    <row r="787" ht="16.5" customHeight="1"/>
+    <row r="788" ht="16.5" customHeight="1"/>
+    <row r="789" ht="16.5" customHeight="1"/>
+    <row r="790" ht="16.5" customHeight="1"/>
+    <row r="791" ht="16.5" customHeight="1"/>
+    <row r="792" ht="16.5" customHeight="1"/>
+    <row r="793" ht="16.5" customHeight="1"/>
+    <row r="794" ht="16.5" customHeight="1"/>
+    <row r="795" ht="16.5" customHeight="1"/>
+    <row r="796" ht="16.5" customHeight="1"/>
+    <row r="797" ht="16.5" customHeight="1"/>
+    <row r="798" ht="16.5" customHeight="1"/>
+    <row r="799" ht="16.5" customHeight="1"/>
+    <row r="800" ht="16.5" customHeight="1"/>
+    <row r="801" ht="16.5" customHeight="1"/>
+    <row r="802" ht="16.5" customHeight="1"/>
+    <row r="803" ht="16.5" customHeight="1"/>
+    <row r="804" ht="16.5" customHeight="1"/>
+    <row r="805" ht="16.5" customHeight="1"/>
+    <row r="806" ht="16.5" customHeight="1"/>
+    <row r="807" ht="16.5" customHeight="1"/>
+    <row r="808" ht="16.5" customHeight="1"/>
+    <row r="809" ht="16.5" customHeight="1"/>
+    <row r="810" ht="16.5" customHeight="1"/>
+    <row r="811" ht="16.5" customHeight="1"/>
+    <row r="812" ht="16.5" customHeight="1"/>
+    <row r="813" ht="16.5" customHeight="1"/>
+    <row r="814" ht="16.5" customHeight="1"/>
+    <row r="815" ht="16.5" customHeight="1"/>
+    <row r="816" ht="16.5" customHeight="1"/>
+    <row r="817" ht="16.5" customHeight="1"/>
+    <row r="818" ht="16.5" customHeight="1"/>
+    <row r="819" ht="16.5" customHeight="1"/>
+    <row r="820" ht="16.5" customHeight="1"/>
+    <row r="821" ht="16.5" customHeight="1"/>
+    <row r="822" ht="16.5" customHeight="1"/>
+    <row r="823" ht="16.5" customHeight="1"/>
+    <row r="824" ht="16.5" customHeight="1"/>
+    <row r="825" ht="16.5" customHeight="1"/>
+    <row r="826" ht="16.5" customHeight="1"/>
+    <row r="827" ht="16.5" customHeight="1"/>
+    <row r="828" ht="16.5" customHeight="1"/>
+    <row r="829" ht="16.5" customHeight="1"/>
+    <row r="830" ht="16.5" customHeight="1"/>
+    <row r="831" ht="16.5" customHeight="1"/>
+    <row r="832" ht="16.5" customHeight="1"/>
+    <row r="833" ht="16.5" customHeight="1"/>
+    <row r="834" ht="16.5" customHeight="1"/>
+    <row r="835" ht="16.5" customHeight="1"/>
+    <row r="836" ht="16.5" customHeight="1"/>
+    <row r="837" ht="16.5" customHeight="1"/>
+    <row r="838" ht="16.5" customHeight="1"/>
+    <row r="839" ht="16.5" customHeight="1"/>
+    <row r="840" ht="16.5" customHeight="1"/>
+    <row r="841" ht="16.5" customHeight="1"/>
+    <row r="842" ht="16.5" customHeight="1"/>
+    <row r="843" ht="16.5" customHeight="1"/>
+    <row r="844" ht="16.5" customHeight="1"/>
+    <row r="845" ht="16.5" customHeight="1"/>
+    <row r="846" ht="16.5" customHeight="1"/>
+    <row r="847" ht="16.5" customHeight="1"/>
+    <row r="848" ht="16.5" customHeight="1"/>
+    <row r="849" ht="16.5" customHeight="1"/>
+    <row r="850" ht="16.5" customHeight="1"/>
+    <row r="851" ht="16.5" customHeight="1"/>
+    <row r="852" ht="16.5" customHeight="1"/>
+    <row r="853" ht="16.5" customHeight="1"/>
+    <row r="854" ht="16.5" customHeight="1"/>
+    <row r="855" ht="16.5" customHeight="1"/>
+    <row r="856" ht="16.5" customHeight="1"/>
+    <row r="857" ht="16.5" customHeight="1"/>
+    <row r="858" ht="16.5" customHeight="1"/>
+    <row r="859" ht="16.5" customHeight="1"/>
+    <row r="860" ht="16.5" customHeight="1"/>
+    <row r="861" ht="16.5" customHeight="1"/>
+    <row r="862" ht="16.5" customHeight="1"/>
+    <row r="863" ht="16.5" customHeight="1"/>
+    <row r="864" ht="16.5" customHeight="1"/>
+    <row r="865" ht="16.5" customHeight="1"/>
+    <row r="866" ht="16.5" customHeight="1"/>
+    <row r="867" ht="16.5" customHeight="1"/>
+    <row r="868" ht="16.5" customHeight="1"/>
+    <row r="869" ht="16.5" customHeight="1"/>
+    <row r="870" ht="16.5" customHeight="1"/>
+    <row r="871" ht="16.5" customHeight="1"/>
+    <row r="872" ht="16.5" customHeight="1"/>
+    <row r="873" ht="16.5" customHeight="1"/>
+    <row r="874" ht="16.5" customHeight="1"/>
+    <row r="875" ht="16.5" customHeight="1"/>
+    <row r="876" ht="16.5" customHeight="1"/>
+    <row r="877" ht="16.5" customHeight="1"/>
+    <row r="878" ht="16.5" customHeight="1"/>
+    <row r="879" ht="16.5" customHeight="1"/>
+    <row r="880" ht="16.5" customHeight="1"/>
+    <row r="881" ht="16.5" customHeight="1"/>
+    <row r="882" ht="16.5" customHeight="1"/>
+    <row r="883" ht="16.5" customHeight="1"/>
+    <row r="884" ht="16.5" customHeight="1"/>
+    <row r="885" ht="16.5" customHeight="1"/>
+    <row r="886" ht="16.5" customHeight="1"/>
+    <row r="887" ht="16.5" customHeight="1"/>
+    <row r="888" ht="16.5" customHeight="1"/>
+    <row r="889" ht="16.5" customHeight="1"/>
+    <row r="890" ht="16.5" customHeight="1"/>
+    <row r="891" ht="16.5" customHeight="1"/>
+    <row r="892" ht="16.5" customHeight="1"/>
+    <row r="893" ht="16.5" customHeight="1"/>
+    <row r="894" ht="16.5" customHeight="1"/>
+    <row r="895" ht="16.5" customHeight="1"/>
+    <row r="896" ht="16.5" customHeight="1"/>
+    <row r="897" ht="16.5" customHeight="1"/>
+    <row r="898" ht="16.5" customHeight="1"/>
+    <row r="899" ht="16.5" customHeight="1"/>
+    <row r="900" ht="16.5" customHeight="1"/>
+    <row r="901" ht="16.5" customHeight="1"/>
+    <row r="902" ht="16.5" customHeight="1"/>
+    <row r="903" ht="16.5" customHeight="1"/>
+    <row r="904" ht="16.5" customHeight="1"/>
+    <row r="905" ht="16.5" customHeight="1"/>
+    <row r="906" ht="16.5" customHeight="1"/>
+    <row r="907" ht="16.5" customHeight="1"/>
+    <row r="908" ht="16.5" customHeight="1"/>
+    <row r="909" ht="16.5" customHeight="1"/>
+    <row r="910" ht="16.5" customHeight="1"/>
+    <row r="911" ht="16.5" customHeight="1"/>
+    <row r="912" ht="16.5" customHeight="1"/>
+    <row r="913" ht="16.5" customHeight="1"/>
+    <row r="914" ht="16.5" customHeight="1"/>
+    <row r="915" ht="16.5" customHeight="1"/>
+    <row r="916" ht="16.5" customHeight="1"/>
+    <row r="917" ht="16.5" customHeight="1"/>
+    <row r="918" ht="16.5" customHeight="1"/>
+    <row r="919" ht="16.5" customHeight="1"/>
+    <row r="920" ht="16.5" customHeight="1"/>
+    <row r="921" ht="16.5" customHeight="1"/>
+    <row r="922" ht="16.5" customHeight="1"/>
+    <row r="923" ht="16.5" customHeight="1"/>
+    <row r="924" ht="16.5" customHeight="1"/>
+    <row r="925" ht="16.5" customHeight="1"/>
+    <row r="926" ht="16.5" customHeight="1"/>
+    <row r="927" ht="16.5" customHeight="1"/>
+    <row r="928" ht="16.5" customHeight="1"/>
+    <row r="929" ht="16.5" customHeight="1"/>
+    <row r="930" ht="16.5" customHeight="1"/>
+    <row r="931" ht="16.5" customHeight="1"/>
+    <row r="932" ht="16.5" customHeight="1"/>
+    <row r="933" ht="16.5" customHeight="1"/>
+    <row r="934" ht="16.5" customHeight="1"/>
+    <row r="935" ht="16.5" customHeight="1"/>
+    <row r="936" ht="16.5" customHeight="1"/>
+    <row r="937" ht="16.5" customHeight="1"/>
+    <row r="938" ht="16.5" customHeight="1"/>
+    <row r="939" ht="16.5" customHeight="1"/>
+    <row r="940" ht="16.5" customHeight="1"/>
+    <row r="941" ht="16.5" customHeight="1"/>
+    <row r="942" ht="16.5" customHeight="1"/>
+    <row r="943" ht="16.5" customHeight="1"/>
+    <row r="944" ht="16.5" customHeight="1"/>
+    <row r="945" ht="16.5" customHeight="1"/>
+    <row r="946" ht="16.5" customHeight="1"/>
+    <row r="947" ht="16.5" customHeight="1"/>
+    <row r="948" ht="16.5" customHeight="1"/>
+    <row r="949" ht="16.5" customHeight="1"/>
+    <row r="950" ht="16.5" customHeight="1"/>
+    <row r="951" ht="16.5" customHeight="1"/>
+    <row r="952" ht="16.5" customHeight="1"/>
+    <row r="953" ht="16.5" customHeight="1"/>
+    <row r="954" ht="16.5" customHeight="1"/>
+    <row r="955" ht="16.5" customHeight="1"/>
+    <row r="956" ht="16.5" customHeight="1"/>
+    <row r="957" ht="16.5" customHeight="1"/>
+    <row r="958" ht="16.5" customHeight="1"/>
+    <row r="959" ht="16.5" customHeight="1"/>
+    <row r="960" ht="16.5" customHeight="1"/>
+    <row r="961" ht="16.5" customHeight="1"/>
+    <row r="962" ht="16.5" customHeight="1"/>
+    <row r="963" ht="16.5" customHeight="1"/>
+    <row r="964" ht="16.5" customHeight="1"/>
+    <row r="965" ht="16.5" customHeight="1"/>
+    <row r="966" ht="16.5" customHeight="1"/>
+    <row r="967" ht="16.5" customHeight="1"/>
+    <row r="968" ht="16.5" customHeight="1"/>
+    <row r="969" ht="16.5" customHeight="1"/>
+    <row r="970" ht="16.5" customHeight="1"/>
+    <row r="971" ht="16.5" customHeight="1"/>
+    <row r="972" ht="16.5" customHeight="1"/>
+    <row r="973" ht="16.5" customHeight="1"/>
+    <row r="974" ht="16.5" customHeight="1"/>
+    <row r="975" ht="16.5" customHeight="1"/>
+    <row r="976" ht="16.5" customHeight="1"/>
+    <row r="977" ht="16.5" customHeight="1"/>
+    <row r="978" ht="16.5" customHeight="1"/>
+    <row r="979" ht="16.5" customHeight="1"/>
+    <row r="980" ht="16.5" customHeight="1"/>
+    <row r="981" ht="16.5" customHeight="1"/>
+    <row r="982" ht="16.5" customHeight="1"/>
+    <row r="983" ht="16.5" customHeight="1"/>
+    <row r="984" ht="16.5" customHeight="1"/>
+    <row r="985" ht="16.5" customHeight="1"/>
+    <row r="986" ht="16.5" customHeight="1"/>
+    <row r="987" ht="16.5" customHeight="1"/>
+    <row r="988" ht="16.5" customHeight="1"/>
+    <row r="989" ht="16.5" customHeight="1"/>
+    <row r="990" ht="16.5" customHeight="1"/>
+    <row r="991" ht="16.5" customHeight="1"/>
+    <row r="992" ht="16.5" customHeight="1"/>
+    <row r="993" ht="16.5" customHeight="1"/>
+    <row r="994" ht="16.5" customHeight="1"/>
+    <row r="995" ht="16.5" customHeight="1"/>
+    <row r="996" ht="16.5" customHeight="1"/>
+    <row r="997" ht="16.5" customHeight="1"/>
+    <row r="998" ht="16.5" customHeight="1"/>
+    <row r="999" ht="16.5" customHeight="1"/>
+    <row r="1000" ht="16.5" customHeight="1"/>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+  </mergeCells>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="2.38"/>
+    <col customWidth="1" min="2" max="2" width="14.38"/>
+    <col customWidth="1" min="3" max="3" width="38.88"/>
+    <col customWidth="1" min="4" max="5" width="28.5"/>
+    <col customWidth="1" min="6" max="6" width="4.88"/>
+    <col customWidth="1" min="7" max="26" width="7.63"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="12.75" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" ht="27.75" customHeight="1">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" ht="27.75" customHeight="1">
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" ht="27.75" customHeight="1">
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" ht="27.75" customHeight="1">
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" ht="27.75" customHeight="1">
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" ht="372.0" customHeight="1">
+      <c r="B7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
     </row>
     <row r="8" ht="16.5" customHeight="1"/>
     <row r="9" ht="16.5" customHeight="1"/>

</xml_diff>

<commit_message>
191211 | DRF API
</commit_message>
<xml_diff>
--- a/[계절학기] 191209_학습계획서_대전_1반_김기은.xlsx
+++ b/[계절학기] 191209_학습계획서_대전_1반_김기은.xlsx
@@ -6,19 +6,20 @@
     <sheet state="visible" name="날짜별 계획 " sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="실적(daily) 19.12.09" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="실적(daily) 19.12.10" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="실적(daily) 19.12.11" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mgYvj+F9v3W6t2MsNxKEMJdnxX0Rg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7miAe5UO0XOlgFySrgjEsVk6oo8PqQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>자기주도학습 계획표</t>
   </si>
@@ -47,22 +48,22 @@
     <t>일정</t>
   </si>
   <si>
-    <t>2019.12.09</t>
+    <t>2019.12.10.</t>
   </si>
   <si>
-    <t>2019.12.10.</t>
+    <t>12/09(월)</t>
   </si>
   <si>
     <t>데일리 목표</t>
   </si>
   <si>
-    <t>자기주도학습 계획 작성</t>
-  </si>
-  <si>
-    <t>12/09(월)</t>
+    <t>2019.12.09</t>
   </si>
   <si>
     <t>DataBase</t>
+  </si>
+  <si>
+    <t>자기주도학습 계획 작성</t>
   </si>
   <si>
     <t>12/10(화)</t>
@@ -86,25 +87,37 @@
     <t>12/19(목)</t>
   </si>
   <si>
-    <t>- Github API에서 레포지토리 데이터 추출 및 Python을 이용하여 원하는 API 재가공</t>
+    <t>알고리즘 DB 제작
+Github API를 이용하여 알고리즘 레포지토리 컨텐츠 확보
+여러 경로에 흩어져 있는 정보들을 python을 이용하여 JSON파일로 재구성
+재구성한 JSON 파일을 Data로 하여 Django에서 모델링 한 후 Data가 잘 올라가는지 테스트</t>
   </si>
   <si>
-    <t xml:space="preserve"> - 자기주도학습 계획 작성</t>
+    <t xml:space="preserve"> 자기주도학습 계획 작성</t>
   </si>
   <si>
-    <t xml:space="preserve"> - DataBase</t>
+    <t>지난 1학기 동안 배운 내용을 보기 좋게 포트폴리오로 작성하는 것을 목표로 하여 계획서를 작성
+Github에 올린 알고리즘 및 학습 내용을 Github API를 이용하여 Crawling하여 원하는 정보를 담은 API 재구성
+Django Rest Framwork를 이용하여 새로운 API 서버를 구축한 후 배포
+Github Page와 Vue.js를 활용하여 정적 Web page 구현</t>
   </si>
   <si>
-    <t>- 서버 구축</t>
+    <t xml:space="preserve"> DataBase</t>
   </si>
   <si>
-    <t xml:space="preserve"> - 배포</t>
+    <t>모델링</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Github Page 제작 및 서버 연동</t>
+    <t>서버 구축</t>
   </si>
   <si>
-    <t xml:space="preserve"> - 디자인</t>
+    <t xml:space="preserve"> 배포</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Github Page 제작 및 서버 연동</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 디자인</t>
   </si>
   <si>
     <t xml:space="preserve">데일리별 
@@ -112,29 +125,26 @@
 (분야 및 키워드) </t>
   </si>
   <si>
-    <t xml:space="preserve"> - 지난 1학기 동안 배운 내용을 보기 좋게 포트폴리오로 작성하는 것을 목표로 하여 계획서를 작성</t>
+    <t>자기 주도학습 계획 작성</t>
   </si>
   <si>
-    <t>- 자기 주도학습 계획 작성</t>
+    <t>풀이한 알고리즘 문제 DB 제작</t>
   </si>
   <si>
-    <t>- 풀이한 알고리즘 문제 DB 제작</t>
+    <t>Django 모델링</t>
   </si>
   <si>
-    <t>- 진행한 프로젝트, TIL 등 DB 제작</t>
+    <t>Django 로직 및 서버 구축</t>
   </si>
   <si>
-    <t>- Django 모델링 및 서버 구축</t>
+    <t xml:space="preserve">Django 서버 AWS 배포 </t>
   </si>
   <si>
-    <t xml:space="preserve">- Django 서버 AWS 배포 </t>
-  </si>
-  <si>
-    <t>- Vue.js를 이용한 정적 페이지 제작
+    <t>Vue.js를 이용한 정적 페이지 제작
 - Django 서버 연동</t>
   </si>
   <si>
-    <t>- Github Page 디자인</t>
+    <t>Github Page 디자인</t>
   </si>
   <si>
     <t xml:space="preserve">활동자료 </t>
@@ -167,16 +177,30 @@
     <t>실행 내용</t>
   </si>
   <si>
-    <t>- Github API에서 레포지토리
+    <t>Github API에서 레포지토리
 데이터 추출 및 Python을 이용하여
 원하는 API 재가공</t>
+  </si>
+  <si>
+    <t>Django Modeling
+Django Rest Framework server 구축
+Vue-CLI 프로젝트 생성</t>
+  </si>
+  <si>
+    <t>2019.12.11.</t>
+  </si>
+  <si>
+    <t>Django Rest Framework에 등록한 API 데이터를 모델링
+fields -&gt; 문제 번호, 출처, 문제명, 난이도, 카테고리, github 문제 url 주소
+Django Rest Framework 구축
+Vue-CLI 프로젝트 생성</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -202,6 +226,10 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
     </font>
   </fonts>
   <fills count="3">
@@ -542,14 +570,14 @@
     <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -616,6 +644,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -875,7 +907,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>15</v>
@@ -900,52 +932,52 @@
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="16" t="s">
+      <c r="D6" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="E6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="F6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="G6" s="18" t="s">
         <v>28</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" ht="39.75" customHeight="1">
       <c r="B7" s="19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" ht="39.75" customHeight="1">
@@ -980,39 +1012,41 @@
     </row>
     <row r="11" ht="143.25" customHeight="1">
       <c r="B11" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" ht="39.75" customHeight="1">
       <c r="B12" s="28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>48</v>
+      </c>
       <c r="F12" s="30"/>
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
@@ -2141,7 +2175,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
@@ -2151,7 +2185,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
@@ -2161,10 +2195,10 @@
         <v>18</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
+        <v>24</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
     </row>
     <row r="8" ht="16.5" customHeight="1"/>
     <row r="9" ht="16.5" customHeight="1"/>
@@ -3254,7 +3288,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
@@ -3264,7 +3298,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
@@ -3276,8 +3310,1121 @@
       <c r="C7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
+    </row>
+    <row r="8" ht="16.5" customHeight="1"/>
+    <row r="9" ht="16.5" customHeight="1"/>
+    <row r="10" ht="16.5" customHeight="1"/>
+    <row r="11" ht="16.5" customHeight="1"/>
+    <row r="12" ht="16.5" customHeight="1"/>
+    <row r="13" ht="16.5" customHeight="1"/>
+    <row r="14" ht="16.5" customHeight="1"/>
+    <row r="15" ht="16.5" customHeight="1"/>
+    <row r="16" ht="16.5" customHeight="1"/>
+    <row r="17" ht="16.5" customHeight="1"/>
+    <row r="18" ht="16.5" customHeight="1"/>
+    <row r="19" ht="16.5" customHeight="1"/>
+    <row r="20" ht="16.5" customHeight="1"/>
+    <row r="21" ht="16.5" customHeight="1"/>
+    <row r="22" ht="16.5" customHeight="1"/>
+    <row r="23" ht="16.5" customHeight="1"/>
+    <row r="24" ht="16.5" customHeight="1"/>
+    <row r="25" ht="16.5" customHeight="1"/>
+    <row r="26" ht="16.5" customHeight="1"/>
+    <row r="27" ht="16.5" customHeight="1"/>
+    <row r="28" ht="16.5" customHeight="1"/>
+    <row r="29" ht="16.5" customHeight="1"/>
+    <row r="30" ht="16.5" customHeight="1"/>
+    <row r="31" ht="16.5" customHeight="1"/>
+    <row r="32" ht="16.5" customHeight="1"/>
+    <row r="33" ht="16.5" customHeight="1"/>
+    <row r="34" ht="16.5" customHeight="1"/>
+    <row r="35" ht="16.5" customHeight="1"/>
+    <row r="36" ht="16.5" customHeight="1"/>
+    <row r="37" ht="16.5" customHeight="1"/>
+    <row r="38" ht="16.5" customHeight="1"/>
+    <row r="39" ht="16.5" customHeight="1"/>
+    <row r="40" ht="16.5" customHeight="1"/>
+    <row r="41" ht="16.5" customHeight="1"/>
+    <row r="42" ht="16.5" customHeight="1"/>
+    <row r="43" ht="16.5" customHeight="1"/>
+    <row r="44" ht="16.5" customHeight="1"/>
+    <row r="45" ht="16.5" customHeight="1"/>
+    <row r="46" ht="16.5" customHeight="1"/>
+    <row r="47" ht="16.5" customHeight="1"/>
+    <row r="48" ht="16.5" customHeight="1"/>
+    <row r="49" ht="16.5" customHeight="1"/>
+    <row r="50" ht="16.5" customHeight="1"/>
+    <row r="51" ht="16.5" customHeight="1"/>
+    <row r="52" ht="16.5" customHeight="1"/>
+    <row r="53" ht="16.5" customHeight="1"/>
+    <row r="54" ht="16.5" customHeight="1"/>
+    <row r="55" ht="16.5" customHeight="1"/>
+    <row r="56" ht="16.5" customHeight="1"/>
+    <row r="57" ht="16.5" customHeight="1"/>
+    <row r="58" ht="16.5" customHeight="1"/>
+    <row r="59" ht="16.5" customHeight="1"/>
+    <row r="60" ht="16.5" customHeight="1"/>
+    <row r="61" ht="16.5" customHeight="1"/>
+    <row r="62" ht="16.5" customHeight="1"/>
+    <row r="63" ht="16.5" customHeight="1"/>
+    <row r="64" ht="16.5" customHeight="1"/>
+    <row r="65" ht="16.5" customHeight="1"/>
+    <row r="66" ht="16.5" customHeight="1"/>
+    <row r="67" ht="16.5" customHeight="1"/>
+    <row r="68" ht="16.5" customHeight="1"/>
+    <row r="69" ht="16.5" customHeight="1"/>
+    <row r="70" ht="16.5" customHeight="1"/>
+    <row r="71" ht="16.5" customHeight="1"/>
+    <row r="72" ht="16.5" customHeight="1"/>
+    <row r="73" ht="16.5" customHeight="1"/>
+    <row r="74" ht="16.5" customHeight="1"/>
+    <row r="75" ht="16.5" customHeight="1"/>
+    <row r="76" ht="16.5" customHeight="1"/>
+    <row r="77" ht="16.5" customHeight="1"/>
+    <row r="78" ht="16.5" customHeight="1"/>
+    <row r="79" ht="16.5" customHeight="1"/>
+    <row r="80" ht="16.5" customHeight="1"/>
+    <row r="81" ht="16.5" customHeight="1"/>
+    <row r="82" ht="16.5" customHeight="1"/>
+    <row r="83" ht="16.5" customHeight="1"/>
+    <row r="84" ht="16.5" customHeight="1"/>
+    <row r="85" ht="16.5" customHeight="1"/>
+    <row r="86" ht="16.5" customHeight="1"/>
+    <row r="87" ht="16.5" customHeight="1"/>
+    <row r="88" ht="16.5" customHeight="1"/>
+    <row r="89" ht="16.5" customHeight="1"/>
+    <row r="90" ht="16.5" customHeight="1"/>
+    <row r="91" ht="16.5" customHeight="1"/>
+    <row r="92" ht="16.5" customHeight="1"/>
+    <row r="93" ht="16.5" customHeight="1"/>
+    <row r="94" ht="16.5" customHeight="1"/>
+    <row r="95" ht="16.5" customHeight="1"/>
+    <row r="96" ht="16.5" customHeight="1"/>
+    <row r="97" ht="16.5" customHeight="1"/>
+    <row r="98" ht="16.5" customHeight="1"/>
+    <row r="99" ht="16.5" customHeight="1"/>
+    <row r="100" ht="16.5" customHeight="1"/>
+    <row r="101" ht="16.5" customHeight="1"/>
+    <row r="102" ht="16.5" customHeight="1"/>
+    <row r="103" ht="16.5" customHeight="1"/>
+    <row r="104" ht="16.5" customHeight="1"/>
+    <row r="105" ht="16.5" customHeight="1"/>
+    <row r="106" ht="16.5" customHeight="1"/>
+    <row r="107" ht="16.5" customHeight="1"/>
+    <row r="108" ht="16.5" customHeight="1"/>
+    <row r="109" ht="16.5" customHeight="1"/>
+    <row r="110" ht="16.5" customHeight="1"/>
+    <row r="111" ht="16.5" customHeight="1"/>
+    <row r="112" ht="16.5" customHeight="1"/>
+    <row r="113" ht="16.5" customHeight="1"/>
+    <row r="114" ht="16.5" customHeight="1"/>
+    <row r="115" ht="16.5" customHeight="1"/>
+    <row r="116" ht="16.5" customHeight="1"/>
+    <row r="117" ht="16.5" customHeight="1"/>
+    <row r="118" ht="16.5" customHeight="1"/>
+    <row r="119" ht="16.5" customHeight="1"/>
+    <row r="120" ht="16.5" customHeight="1"/>
+    <row r="121" ht="16.5" customHeight="1"/>
+    <row r="122" ht="16.5" customHeight="1"/>
+    <row r="123" ht="16.5" customHeight="1"/>
+    <row r="124" ht="16.5" customHeight="1"/>
+    <row r="125" ht="16.5" customHeight="1"/>
+    <row r="126" ht="16.5" customHeight="1"/>
+    <row r="127" ht="16.5" customHeight="1"/>
+    <row r="128" ht="16.5" customHeight="1"/>
+    <row r="129" ht="16.5" customHeight="1"/>
+    <row r="130" ht="16.5" customHeight="1"/>
+    <row r="131" ht="16.5" customHeight="1"/>
+    <row r="132" ht="16.5" customHeight="1"/>
+    <row r="133" ht="16.5" customHeight="1"/>
+    <row r="134" ht="16.5" customHeight="1"/>
+    <row r="135" ht="16.5" customHeight="1"/>
+    <row r="136" ht="16.5" customHeight="1"/>
+    <row r="137" ht="16.5" customHeight="1"/>
+    <row r="138" ht="16.5" customHeight="1"/>
+    <row r="139" ht="16.5" customHeight="1"/>
+    <row r="140" ht="16.5" customHeight="1"/>
+    <row r="141" ht="16.5" customHeight="1"/>
+    <row r="142" ht="16.5" customHeight="1"/>
+    <row r="143" ht="16.5" customHeight="1"/>
+    <row r="144" ht="16.5" customHeight="1"/>
+    <row r="145" ht="16.5" customHeight="1"/>
+    <row r="146" ht="16.5" customHeight="1"/>
+    <row r="147" ht="16.5" customHeight="1"/>
+    <row r="148" ht="16.5" customHeight="1"/>
+    <row r="149" ht="16.5" customHeight="1"/>
+    <row r="150" ht="16.5" customHeight="1"/>
+    <row r="151" ht="16.5" customHeight="1"/>
+    <row r="152" ht="16.5" customHeight="1"/>
+    <row r="153" ht="16.5" customHeight="1"/>
+    <row r="154" ht="16.5" customHeight="1"/>
+    <row r="155" ht="16.5" customHeight="1"/>
+    <row r="156" ht="16.5" customHeight="1"/>
+    <row r="157" ht="16.5" customHeight="1"/>
+    <row r="158" ht="16.5" customHeight="1"/>
+    <row r="159" ht="16.5" customHeight="1"/>
+    <row r="160" ht="16.5" customHeight="1"/>
+    <row r="161" ht="16.5" customHeight="1"/>
+    <row r="162" ht="16.5" customHeight="1"/>
+    <row r="163" ht="16.5" customHeight="1"/>
+    <row r="164" ht="16.5" customHeight="1"/>
+    <row r="165" ht="16.5" customHeight="1"/>
+    <row r="166" ht="16.5" customHeight="1"/>
+    <row r="167" ht="16.5" customHeight="1"/>
+    <row r="168" ht="16.5" customHeight="1"/>
+    <row r="169" ht="16.5" customHeight="1"/>
+    <row r="170" ht="16.5" customHeight="1"/>
+    <row r="171" ht="16.5" customHeight="1"/>
+    <row r="172" ht="16.5" customHeight="1"/>
+    <row r="173" ht="16.5" customHeight="1"/>
+    <row r="174" ht="16.5" customHeight="1"/>
+    <row r="175" ht="16.5" customHeight="1"/>
+    <row r="176" ht="16.5" customHeight="1"/>
+    <row r="177" ht="16.5" customHeight="1"/>
+    <row r="178" ht="16.5" customHeight="1"/>
+    <row r="179" ht="16.5" customHeight="1"/>
+    <row r="180" ht="16.5" customHeight="1"/>
+    <row r="181" ht="16.5" customHeight="1"/>
+    <row r="182" ht="16.5" customHeight="1"/>
+    <row r="183" ht="16.5" customHeight="1"/>
+    <row r="184" ht="16.5" customHeight="1"/>
+    <row r="185" ht="16.5" customHeight="1"/>
+    <row r="186" ht="16.5" customHeight="1"/>
+    <row r="187" ht="16.5" customHeight="1"/>
+    <row r="188" ht="16.5" customHeight="1"/>
+    <row r="189" ht="16.5" customHeight="1"/>
+    <row r="190" ht="16.5" customHeight="1"/>
+    <row r="191" ht="16.5" customHeight="1"/>
+    <row r="192" ht="16.5" customHeight="1"/>
+    <row r="193" ht="16.5" customHeight="1"/>
+    <row r="194" ht="16.5" customHeight="1"/>
+    <row r="195" ht="16.5" customHeight="1"/>
+    <row r="196" ht="16.5" customHeight="1"/>
+    <row r="197" ht="16.5" customHeight="1"/>
+    <row r="198" ht="16.5" customHeight="1"/>
+    <row r="199" ht="16.5" customHeight="1"/>
+    <row r="200" ht="16.5" customHeight="1"/>
+    <row r="201" ht="16.5" customHeight="1"/>
+    <row r="202" ht="16.5" customHeight="1"/>
+    <row r="203" ht="16.5" customHeight="1"/>
+    <row r="204" ht="16.5" customHeight="1"/>
+    <row r="205" ht="16.5" customHeight="1"/>
+    <row r="206" ht="16.5" customHeight="1"/>
+    <row r="207" ht="16.5" customHeight="1"/>
+    <row r="208" ht="16.5" customHeight="1"/>
+    <row r="209" ht="16.5" customHeight="1"/>
+    <row r="210" ht="16.5" customHeight="1"/>
+    <row r="211" ht="16.5" customHeight="1"/>
+    <row r="212" ht="16.5" customHeight="1"/>
+    <row r="213" ht="16.5" customHeight="1"/>
+    <row r="214" ht="16.5" customHeight="1"/>
+    <row r="215" ht="16.5" customHeight="1"/>
+    <row r="216" ht="16.5" customHeight="1"/>
+    <row r="217" ht="16.5" customHeight="1"/>
+    <row r="218" ht="16.5" customHeight="1"/>
+    <row r="219" ht="16.5" customHeight="1"/>
+    <row r="220" ht="16.5" customHeight="1"/>
+    <row r="221" ht="16.5" customHeight="1"/>
+    <row r="222" ht="16.5" customHeight="1"/>
+    <row r="223" ht="16.5" customHeight="1"/>
+    <row r="224" ht="16.5" customHeight="1"/>
+    <row r="225" ht="16.5" customHeight="1"/>
+    <row r="226" ht="16.5" customHeight="1"/>
+    <row r="227" ht="16.5" customHeight="1"/>
+    <row r="228" ht="16.5" customHeight="1"/>
+    <row r="229" ht="16.5" customHeight="1"/>
+    <row r="230" ht="16.5" customHeight="1"/>
+    <row r="231" ht="16.5" customHeight="1"/>
+    <row r="232" ht="16.5" customHeight="1"/>
+    <row r="233" ht="16.5" customHeight="1"/>
+    <row r="234" ht="16.5" customHeight="1"/>
+    <row r="235" ht="16.5" customHeight="1"/>
+    <row r="236" ht="16.5" customHeight="1"/>
+    <row r="237" ht="16.5" customHeight="1"/>
+    <row r="238" ht="16.5" customHeight="1"/>
+    <row r="239" ht="16.5" customHeight="1"/>
+    <row r="240" ht="16.5" customHeight="1"/>
+    <row r="241" ht="16.5" customHeight="1"/>
+    <row r="242" ht="16.5" customHeight="1"/>
+    <row r="243" ht="16.5" customHeight="1"/>
+    <row r="244" ht="16.5" customHeight="1"/>
+    <row r="245" ht="16.5" customHeight="1"/>
+    <row r="246" ht="16.5" customHeight="1"/>
+    <row r="247" ht="16.5" customHeight="1"/>
+    <row r="248" ht="16.5" customHeight="1"/>
+    <row r="249" ht="16.5" customHeight="1"/>
+    <row r="250" ht="16.5" customHeight="1"/>
+    <row r="251" ht="16.5" customHeight="1"/>
+    <row r="252" ht="16.5" customHeight="1"/>
+    <row r="253" ht="16.5" customHeight="1"/>
+    <row r="254" ht="16.5" customHeight="1"/>
+    <row r="255" ht="16.5" customHeight="1"/>
+    <row r="256" ht="16.5" customHeight="1"/>
+    <row r="257" ht="16.5" customHeight="1"/>
+    <row r="258" ht="16.5" customHeight="1"/>
+    <row r="259" ht="16.5" customHeight="1"/>
+    <row r="260" ht="16.5" customHeight="1"/>
+    <row r="261" ht="16.5" customHeight="1"/>
+    <row r="262" ht="16.5" customHeight="1"/>
+    <row r="263" ht="16.5" customHeight="1"/>
+    <row r="264" ht="16.5" customHeight="1"/>
+    <row r="265" ht="16.5" customHeight="1"/>
+    <row r="266" ht="16.5" customHeight="1"/>
+    <row r="267" ht="16.5" customHeight="1"/>
+    <row r="268" ht="16.5" customHeight="1"/>
+    <row r="269" ht="16.5" customHeight="1"/>
+    <row r="270" ht="16.5" customHeight="1"/>
+    <row r="271" ht="16.5" customHeight="1"/>
+    <row r="272" ht="16.5" customHeight="1"/>
+    <row r="273" ht="16.5" customHeight="1"/>
+    <row r="274" ht="16.5" customHeight="1"/>
+    <row r="275" ht="16.5" customHeight="1"/>
+    <row r="276" ht="16.5" customHeight="1"/>
+    <row r="277" ht="16.5" customHeight="1"/>
+    <row r="278" ht="16.5" customHeight="1"/>
+    <row r="279" ht="16.5" customHeight="1"/>
+    <row r="280" ht="16.5" customHeight="1"/>
+    <row r="281" ht="16.5" customHeight="1"/>
+    <row r="282" ht="16.5" customHeight="1"/>
+    <row r="283" ht="16.5" customHeight="1"/>
+    <row r="284" ht="16.5" customHeight="1"/>
+    <row r="285" ht="16.5" customHeight="1"/>
+    <row r="286" ht="16.5" customHeight="1"/>
+    <row r="287" ht="16.5" customHeight="1"/>
+    <row r="288" ht="16.5" customHeight="1"/>
+    <row r="289" ht="16.5" customHeight="1"/>
+    <row r="290" ht="16.5" customHeight="1"/>
+    <row r="291" ht="16.5" customHeight="1"/>
+    <row r="292" ht="16.5" customHeight="1"/>
+    <row r="293" ht="16.5" customHeight="1"/>
+    <row r="294" ht="16.5" customHeight="1"/>
+    <row r="295" ht="16.5" customHeight="1"/>
+    <row r="296" ht="16.5" customHeight="1"/>
+    <row r="297" ht="16.5" customHeight="1"/>
+    <row r="298" ht="16.5" customHeight="1"/>
+    <row r="299" ht="16.5" customHeight="1"/>
+    <row r="300" ht="16.5" customHeight="1"/>
+    <row r="301" ht="16.5" customHeight="1"/>
+    <row r="302" ht="16.5" customHeight="1"/>
+    <row r="303" ht="16.5" customHeight="1"/>
+    <row r="304" ht="16.5" customHeight="1"/>
+    <row r="305" ht="16.5" customHeight="1"/>
+    <row r="306" ht="16.5" customHeight="1"/>
+    <row r="307" ht="16.5" customHeight="1"/>
+    <row r="308" ht="16.5" customHeight="1"/>
+    <row r="309" ht="16.5" customHeight="1"/>
+    <row r="310" ht="16.5" customHeight="1"/>
+    <row r="311" ht="16.5" customHeight="1"/>
+    <row r="312" ht="16.5" customHeight="1"/>
+    <row r="313" ht="16.5" customHeight="1"/>
+    <row r="314" ht="16.5" customHeight="1"/>
+    <row r="315" ht="16.5" customHeight="1"/>
+    <row r="316" ht="16.5" customHeight="1"/>
+    <row r="317" ht="16.5" customHeight="1"/>
+    <row r="318" ht="16.5" customHeight="1"/>
+    <row r="319" ht="16.5" customHeight="1"/>
+    <row r="320" ht="16.5" customHeight="1"/>
+    <row r="321" ht="16.5" customHeight="1"/>
+    <row r="322" ht="16.5" customHeight="1"/>
+    <row r="323" ht="16.5" customHeight="1"/>
+    <row r="324" ht="16.5" customHeight="1"/>
+    <row r="325" ht="16.5" customHeight="1"/>
+    <row r="326" ht="16.5" customHeight="1"/>
+    <row r="327" ht="16.5" customHeight="1"/>
+    <row r="328" ht="16.5" customHeight="1"/>
+    <row r="329" ht="16.5" customHeight="1"/>
+    <row r="330" ht="16.5" customHeight="1"/>
+    <row r="331" ht="16.5" customHeight="1"/>
+    <row r="332" ht="16.5" customHeight="1"/>
+    <row r="333" ht="16.5" customHeight="1"/>
+    <row r="334" ht="16.5" customHeight="1"/>
+    <row r="335" ht="16.5" customHeight="1"/>
+    <row r="336" ht="16.5" customHeight="1"/>
+    <row r="337" ht="16.5" customHeight="1"/>
+    <row r="338" ht="16.5" customHeight="1"/>
+    <row r="339" ht="16.5" customHeight="1"/>
+    <row r="340" ht="16.5" customHeight="1"/>
+    <row r="341" ht="16.5" customHeight="1"/>
+    <row r="342" ht="16.5" customHeight="1"/>
+    <row r="343" ht="16.5" customHeight="1"/>
+    <row r="344" ht="16.5" customHeight="1"/>
+    <row r="345" ht="16.5" customHeight="1"/>
+    <row r="346" ht="16.5" customHeight="1"/>
+    <row r="347" ht="16.5" customHeight="1"/>
+    <row r="348" ht="16.5" customHeight="1"/>
+    <row r="349" ht="16.5" customHeight="1"/>
+    <row r="350" ht="16.5" customHeight="1"/>
+    <row r="351" ht="16.5" customHeight="1"/>
+    <row r="352" ht="16.5" customHeight="1"/>
+    <row r="353" ht="16.5" customHeight="1"/>
+    <row r="354" ht="16.5" customHeight="1"/>
+    <row r="355" ht="16.5" customHeight="1"/>
+    <row r="356" ht="16.5" customHeight="1"/>
+    <row r="357" ht="16.5" customHeight="1"/>
+    <row r="358" ht="16.5" customHeight="1"/>
+    <row r="359" ht="16.5" customHeight="1"/>
+    <row r="360" ht="16.5" customHeight="1"/>
+    <row r="361" ht="16.5" customHeight="1"/>
+    <row r="362" ht="16.5" customHeight="1"/>
+    <row r="363" ht="16.5" customHeight="1"/>
+    <row r="364" ht="16.5" customHeight="1"/>
+    <row r="365" ht="16.5" customHeight="1"/>
+    <row r="366" ht="16.5" customHeight="1"/>
+    <row r="367" ht="16.5" customHeight="1"/>
+    <row r="368" ht="16.5" customHeight="1"/>
+    <row r="369" ht="16.5" customHeight="1"/>
+    <row r="370" ht="16.5" customHeight="1"/>
+    <row r="371" ht="16.5" customHeight="1"/>
+    <row r="372" ht="16.5" customHeight="1"/>
+    <row r="373" ht="16.5" customHeight="1"/>
+    <row r="374" ht="16.5" customHeight="1"/>
+    <row r="375" ht="16.5" customHeight="1"/>
+    <row r="376" ht="16.5" customHeight="1"/>
+    <row r="377" ht="16.5" customHeight="1"/>
+    <row r="378" ht="16.5" customHeight="1"/>
+    <row r="379" ht="16.5" customHeight="1"/>
+    <row r="380" ht="16.5" customHeight="1"/>
+    <row r="381" ht="16.5" customHeight="1"/>
+    <row r="382" ht="16.5" customHeight="1"/>
+    <row r="383" ht="16.5" customHeight="1"/>
+    <row r="384" ht="16.5" customHeight="1"/>
+    <row r="385" ht="16.5" customHeight="1"/>
+    <row r="386" ht="16.5" customHeight="1"/>
+    <row r="387" ht="16.5" customHeight="1"/>
+    <row r="388" ht="16.5" customHeight="1"/>
+    <row r="389" ht="16.5" customHeight="1"/>
+    <row r="390" ht="16.5" customHeight="1"/>
+    <row r="391" ht="16.5" customHeight="1"/>
+    <row r="392" ht="16.5" customHeight="1"/>
+    <row r="393" ht="16.5" customHeight="1"/>
+    <row r="394" ht="16.5" customHeight="1"/>
+    <row r="395" ht="16.5" customHeight="1"/>
+    <row r="396" ht="16.5" customHeight="1"/>
+    <row r="397" ht="16.5" customHeight="1"/>
+    <row r="398" ht="16.5" customHeight="1"/>
+    <row r="399" ht="16.5" customHeight="1"/>
+    <row r="400" ht="16.5" customHeight="1"/>
+    <row r="401" ht="16.5" customHeight="1"/>
+    <row r="402" ht="16.5" customHeight="1"/>
+    <row r="403" ht="16.5" customHeight="1"/>
+    <row r="404" ht="16.5" customHeight="1"/>
+    <row r="405" ht="16.5" customHeight="1"/>
+    <row r="406" ht="16.5" customHeight="1"/>
+    <row r="407" ht="16.5" customHeight="1"/>
+    <row r="408" ht="16.5" customHeight="1"/>
+    <row r="409" ht="16.5" customHeight="1"/>
+    <row r="410" ht="16.5" customHeight="1"/>
+    <row r="411" ht="16.5" customHeight="1"/>
+    <row r="412" ht="16.5" customHeight="1"/>
+    <row r="413" ht="16.5" customHeight="1"/>
+    <row r="414" ht="16.5" customHeight="1"/>
+    <row r="415" ht="16.5" customHeight="1"/>
+    <row r="416" ht="16.5" customHeight="1"/>
+    <row r="417" ht="16.5" customHeight="1"/>
+    <row r="418" ht="16.5" customHeight="1"/>
+    <row r="419" ht="16.5" customHeight="1"/>
+    <row r="420" ht="16.5" customHeight="1"/>
+    <row r="421" ht="16.5" customHeight="1"/>
+    <row r="422" ht="16.5" customHeight="1"/>
+    <row r="423" ht="16.5" customHeight="1"/>
+    <row r="424" ht="16.5" customHeight="1"/>
+    <row r="425" ht="16.5" customHeight="1"/>
+    <row r="426" ht="16.5" customHeight="1"/>
+    <row r="427" ht="16.5" customHeight="1"/>
+    <row r="428" ht="16.5" customHeight="1"/>
+    <row r="429" ht="16.5" customHeight="1"/>
+    <row r="430" ht="16.5" customHeight="1"/>
+    <row r="431" ht="16.5" customHeight="1"/>
+    <row r="432" ht="16.5" customHeight="1"/>
+    <row r="433" ht="16.5" customHeight="1"/>
+    <row r="434" ht="16.5" customHeight="1"/>
+    <row r="435" ht="16.5" customHeight="1"/>
+    <row r="436" ht="16.5" customHeight="1"/>
+    <row r="437" ht="16.5" customHeight="1"/>
+    <row r="438" ht="16.5" customHeight="1"/>
+    <row r="439" ht="16.5" customHeight="1"/>
+    <row r="440" ht="16.5" customHeight="1"/>
+    <row r="441" ht="16.5" customHeight="1"/>
+    <row r="442" ht="16.5" customHeight="1"/>
+    <row r="443" ht="16.5" customHeight="1"/>
+    <row r="444" ht="16.5" customHeight="1"/>
+    <row r="445" ht="16.5" customHeight="1"/>
+    <row r="446" ht="16.5" customHeight="1"/>
+    <row r="447" ht="16.5" customHeight="1"/>
+    <row r="448" ht="16.5" customHeight="1"/>
+    <row r="449" ht="16.5" customHeight="1"/>
+    <row r="450" ht="16.5" customHeight="1"/>
+    <row r="451" ht="16.5" customHeight="1"/>
+    <row r="452" ht="16.5" customHeight="1"/>
+    <row r="453" ht="16.5" customHeight="1"/>
+    <row r="454" ht="16.5" customHeight="1"/>
+    <row r="455" ht="16.5" customHeight="1"/>
+    <row r="456" ht="16.5" customHeight="1"/>
+    <row r="457" ht="16.5" customHeight="1"/>
+    <row r="458" ht="16.5" customHeight="1"/>
+    <row r="459" ht="16.5" customHeight="1"/>
+    <row r="460" ht="16.5" customHeight="1"/>
+    <row r="461" ht="16.5" customHeight="1"/>
+    <row r="462" ht="16.5" customHeight="1"/>
+    <row r="463" ht="16.5" customHeight="1"/>
+    <row r="464" ht="16.5" customHeight="1"/>
+    <row r="465" ht="16.5" customHeight="1"/>
+    <row r="466" ht="16.5" customHeight="1"/>
+    <row r="467" ht="16.5" customHeight="1"/>
+    <row r="468" ht="16.5" customHeight="1"/>
+    <row r="469" ht="16.5" customHeight="1"/>
+    <row r="470" ht="16.5" customHeight="1"/>
+    <row r="471" ht="16.5" customHeight="1"/>
+    <row r="472" ht="16.5" customHeight="1"/>
+    <row r="473" ht="16.5" customHeight="1"/>
+    <row r="474" ht="16.5" customHeight="1"/>
+    <row r="475" ht="16.5" customHeight="1"/>
+    <row r="476" ht="16.5" customHeight="1"/>
+    <row r="477" ht="16.5" customHeight="1"/>
+    <row r="478" ht="16.5" customHeight="1"/>
+    <row r="479" ht="16.5" customHeight="1"/>
+    <row r="480" ht="16.5" customHeight="1"/>
+    <row r="481" ht="16.5" customHeight="1"/>
+    <row r="482" ht="16.5" customHeight="1"/>
+    <row r="483" ht="16.5" customHeight="1"/>
+    <row r="484" ht="16.5" customHeight="1"/>
+    <row r="485" ht="16.5" customHeight="1"/>
+    <row r="486" ht="16.5" customHeight="1"/>
+    <row r="487" ht="16.5" customHeight="1"/>
+    <row r="488" ht="16.5" customHeight="1"/>
+    <row r="489" ht="16.5" customHeight="1"/>
+    <row r="490" ht="16.5" customHeight="1"/>
+    <row r="491" ht="16.5" customHeight="1"/>
+    <row r="492" ht="16.5" customHeight="1"/>
+    <row r="493" ht="16.5" customHeight="1"/>
+    <row r="494" ht="16.5" customHeight="1"/>
+    <row r="495" ht="16.5" customHeight="1"/>
+    <row r="496" ht="16.5" customHeight="1"/>
+    <row r="497" ht="16.5" customHeight="1"/>
+    <row r="498" ht="16.5" customHeight="1"/>
+    <row r="499" ht="16.5" customHeight="1"/>
+    <row r="500" ht="16.5" customHeight="1"/>
+    <row r="501" ht="16.5" customHeight="1"/>
+    <row r="502" ht="16.5" customHeight="1"/>
+    <row r="503" ht="16.5" customHeight="1"/>
+    <row r="504" ht="16.5" customHeight="1"/>
+    <row r="505" ht="16.5" customHeight="1"/>
+    <row r="506" ht="16.5" customHeight="1"/>
+    <row r="507" ht="16.5" customHeight="1"/>
+    <row r="508" ht="16.5" customHeight="1"/>
+    <row r="509" ht="16.5" customHeight="1"/>
+    <row r="510" ht="16.5" customHeight="1"/>
+    <row r="511" ht="16.5" customHeight="1"/>
+    <row r="512" ht="16.5" customHeight="1"/>
+    <row r="513" ht="16.5" customHeight="1"/>
+    <row r="514" ht="16.5" customHeight="1"/>
+    <row r="515" ht="16.5" customHeight="1"/>
+    <row r="516" ht="16.5" customHeight="1"/>
+    <row r="517" ht="16.5" customHeight="1"/>
+    <row r="518" ht="16.5" customHeight="1"/>
+    <row r="519" ht="16.5" customHeight="1"/>
+    <row r="520" ht="16.5" customHeight="1"/>
+    <row r="521" ht="16.5" customHeight="1"/>
+    <row r="522" ht="16.5" customHeight="1"/>
+    <row r="523" ht="16.5" customHeight="1"/>
+    <row r="524" ht="16.5" customHeight="1"/>
+    <row r="525" ht="16.5" customHeight="1"/>
+    <row r="526" ht="16.5" customHeight="1"/>
+    <row r="527" ht="16.5" customHeight="1"/>
+    <row r="528" ht="16.5" customHeight="1"/>
+    <row r="529" ht="16.5" customHeight="1"/>
+    <row r="530" ht="16.5" customHeight="1"/>
+    <row r="531" ht="16.5" customHeight="1"/>
+    <row r="532" ht="16.5" customHeight="1"/>
+    <row r="533" ht="16.5" customHeight="1"/>
+    <row r="534" ht="16.5" customHeight="1"/>
+    <row r="535" ht="16.5" customHeight="1"/>
+    <row r="536" ht="16.5" customHeight="1"/>
+    <row r="537" ht="16.5" customHeight="1"/>
+    <row r="538" ht="16.5" customHeight="1"/>
+    <row r="539" ht="16.5" customHeight="1"/>
+    <row r="540" ht="16.5" customHeight="1"/>
+    <row r="541" ht="16.5" customHeight="1"/>
+    <row r="542" ht="16.5" customHeight="1"/>
+    <row r="543" ht="16.5" customHeight="1"/>
+    <row r="544" ht="16.5" customHeight="1"/>
+    <row r="545" ht="16.5" customHeight="1"/>
+    <row r="546" ht="16.5" customHeight="1"/>
+    <row r="547" ht="16.5" customHeight="1"/>
+    <row r="548" ht="16.5" customHeight="1"/>
+    <row r="549" ht="16.5" customHeight="1"/>
+    <row r="550" ht="16.5" customHeight="1"/>
+    <row r="551" ht="16.5" customHeight="1"/>
+    <row r="552" ht="16.5" customHeight="1"/>
+    <row r="553" ht="16.5" customHeight="1"/>
+    <row r="554" ht="16.5" customHeight="1"/>
+    <row r="555" ht="16.5" customHeight="1"/>
+    <row r="556" ht="16.5" customHeight="1"/>
+    <row r="557" ht="16.5" customHeight="1"/>
+    <row r="558" ht="16.5" customHeight="1"/>
+    <row r="559" ht="16.5" customHeight="1"/>
+    <row r="560" ht="16.5" customHeight="1"/>
+    <row r="561" ht="16.5" customHeight="1"/>
+    <row r="562" ht="16.5" customHeight="1"/>
+    <row r="563" ht="16.5" customHeight="1"/>
+    <row r="564" ht="16.5" customHeight="1"/>
+    <row r="565" ht="16.5" customHeight="1"/>
+    <row r="566" ht="16.5" customHeight="1"/>
+    <row r="567" ht="16.5" customHeight="1"/>
+    <row r="568" ht="16.5" customHeight="1"/>
+    <row r="569" ht="16.5" customHeight="1"/>
+    <row r="570" ht="16.5" customHeight="1"/>
+    <row r="571" ht="16.5" customHeight="1"/>
+    <row r="572" ht="16.5" customHeight="1"/>
+    <row r="573" ht="16.5" customHeight="1"/>
+    <row r="574" ht="16.5" customHeight="1"/>
+    <row r="575" ht="16.5" customHeight="1"/>
+    <row r="576" ht="16.5" customHeight="1"/>
+    <row r="577" ht="16.5" customHeight="1"/>
+    <row r="578" ht="16.5" customHeight="1"/>
+    <row r="579" ht="16.5" customHeight="1"/>
+    <row r="580" ht="16.5" customHeight="1"/>
+    <row r="581" ht="16.5" customHeight="1"/>
+    <row r="582" ht="16.5" customHeight="1"/>
+    <row r="583" ht="16.5" customHeight="1"/>
+    <row r="584" ht="16.5" customHeight="1"/>
+    <row r="585" ht="16.5" customHeight="1"/>
+    <row r="586" ht="16.5" customHeight="1"/>
+    <row r="587" ht="16.5" customHeight="1"/>
+    <row r="588" ht="16.5" customHeight="1"/>
+    <row r="589" ht="16.5" customHeight="1"/>
+    <row r="590" ht="16.5" customHeight="1"/>
+    <row r="591" ht="16.5" customHeight="1"/>
+    <row r="592" ht="16.5" customHeight="1"/>
+    <row r="593" ht="16.5" customHeight="1"/>
+    <row r="594" ht="16.5" customHeight="1"/>
+    <row r="595" ht="16.5" customHeight="1"/>
+    <row r="596" ht="16.5" customHeight="1"/>
+    <row r="597" ht="16.5" customHeight="1"/>
+    <row r="598" ht="16.5" customHeight="1"/>
+    <row r="599" ht="16.5" customHeight="1"/>
+    <row r="600" ht="16.5" customHeight="1"/>
+    <row r="601" ht="16.5" customHeight="1"/>
+    <row r="602" ht="16.5" customHeight="1"/>
+    <row r="603" ht="16.5" customHeight="1"/>
+    <row r="604" ht="16.5" customHeight="1"/>
+    <row r="605" ht="16.5" customHeight="1"/>
+    <row r="606" ht="16.5" customHeight="1"/>
+    <row r="607" ht="16.5" customHeight="1"/>
+    <row r="608" ht="16.5" customHeight="1"/>
+    <row r="609" ht="16.5" customHeight="1"/>
+    <row r="610" ht="16.5" customHeight="1"/>
+    <row r="611" ht="16.5" customHeight="1"/>
+    <row r="612" ht="16.5" customHeight="1"/>
+    <row r="613" ht="16.5" customHeight="1"/>
+    <row r="614" ht="16.5" customHeight="1"/>
+    <row r="615" ht="16.5" customHeight="1"/>
+    <row r="616" ht="16.5" customHeight="1"/>
+    <row r="617" ht="16.5" customHeight="1"/>
+    <row r="618" ht="16.5" customHeight="1"/>
+    <row r="619" ht="16.5" customHeight="1"/>
+    <row r="620" ht="16.5" customHeight="1"/>
+    <row r="621" ht="16.5" customHeight="1"/>
+    <row r="622" ht="16.5" customHeight="1"/>
+    <row r="623" ht="16.5" customHeight="1"/>
+    <row r="624" ht="16.5" customHeight="1"/>
+    <row r="625" ht="16.5" customHeight="1"/>
+    <row r="626" ht="16.5" customHeight="1"/>
+    <row r="627" ht="16.5" customHeight="1"/>
+    <row r="628" ht="16.5" customHeight="1"/>
+    <row r="629" ht="16.5" customHeight="1"/>
+    <row r="630" ht="16.5" customHeight="1"/>
+    <row r="631" ht="16.5" customHeight="1"/>
+    <row r="632" ht="16.5" customHeight="1"/>
+    <row r="633" ht="16.5" customHeight="1"/>
+    <row r="634" ht="16.5" customHeight="1"/>
+    <row r="635" ht="16.5" customHeight="1"/>
+    <row r="636" ht="16.5" customHeight="1"/>
+    <row r="637" ht="16.5" customHeight="1"/>
+    <row r="638" ht="16.5" customHeight="1"/>
+    <row r="639" ht="16.5" customHeight="1"/>
+    <row r="640" ht="16.5" customHeight="1"/>
+    <row r="641" ht="16.5" customHeight="1"/>
+    <row r="642" ht="16.5" customHeight="1"/>
+    <row r="643" ht="16.5" customHeight="1"/>
+    <row r="644" ht="16.5" customHeight="1"/>
+    <row r="645" ht="16.5" customHeight="1"/>
+    <row r="646" ht="16.5" customHeight="1"/>
+    <row r="647" ht="16.5" customHeight="1"/>
+    <row r="648" ht="16.5" customHeight="1"/>
+    <row r="649" ht="16.5" customHeight="1"/>
+    <row r="650" ht="16.5" customHeight="1"/>
+    <row r="651" ht="16.5" customHeight="1"/>
+    <row r="652" ht="16.5" customHeight="1"/>
+    <row r="653" ht="16.5" customHeight="1"/>
+    <row r="654" ht="16.5" customHeight="1"/>
+    <row r="655" ht="16.5" customHeight="1"/>
+    <row r="656" ht="16.5" customHeight="1"/>
+    <row r="657" ht="16.5" customHeight="1"/>
+    <row r="658" ht="16.5" customHeight="1"/>
+    <row r="659" ht="16.5" customHeight="1"/>
+    <row r="660" ht="16.5" customHeight="1"/>
+    <row r="661" ht="16.5" customHeight="1"/>
+    <row r="662" ht="16.5" customHeight="1"/>
+    <row r="663" ht="16.5" customHeight="1"/>
+    <row r="664" ht="16.5" customHeight="1"/>
+    <row r="665" ht="16.5" customHeight="1"/>
+    <row r="666" ht="16.5" customHeight="1"/>
+    <row r="667" ht="16.5" customHeight="1"/>
+    <row r="668" ht="16.5" customHeight="1"/>
+    <row r="669" ht="16.5" customHeight="1"/>
+    <row r="670" ht="16.5" customHeight="1"/>
+    <row r="671" ht="16.5" customHeight="1"/>
+    <row r="672" ht="16.5" customHeight="1"/>
+    <row r="673" ht="16.5" customHeight="1"/>
+    <row r="674" ht="16.5" customHeight="1"/>
+    <row r="675" ht="16.5" customHeight="1"/>
+    <row r="676" ht="16.5" customHeight="1"/>
+    <row r="677" ht="16.5" customHeight="1"/>
+    <row r="678" ht="16.5" customHeight="1"/>
+    <row r="679" ht="16.5" customHeight="1"/>
+    <row r="680" ht="16.5" customHeight="1"/>
+    <row r="681" ht="16.5" customHeight="1"/>
+    <row r="682" ht="16.5" customHeight="1"/>
+    <row r="683" ht="16.5" customHeight="1"/>
+    <row r="684" ht="16.5" customHeight="1"/>
+    <row r="685" ht="16.5" customHeight="1"/>
+    <row r="686" ht="16.5" customHeight="1"/>
+    <row r="687" ht="16.5" customHeight="1"/>
+    <row r="688" ht="16.5" customHeight="1"/>
+    <row r="689" ht="16.5" customHeight="1"/>
+    <row r="690" ht="16.5" customHeight="1"/>
+    <row r="691" ht="16.5" customHeight="1"/>
+    <row r="692" ht="16.5" customHeight="1"/>
+    <row r="693" ht="16.5" customHeight="1"/>
+    <row r="694" ht="16.5" customHeight="1"/>
+    <row r="695" ht="16.5" customHeight="1"/>
+    <row r="696" ht="16.5" customHeight="1"/>
+    <row r="697" ht="16.5" customHeight="1"/>
+    <row r="698" ht="16.5" customHeight="1"/>
+    <row r="699" ht="16.5" customHeight="1"/>
+    <row r="700" ht="16.5" customHeight="1"/>
+    <row r="701" ht="16.5" customHeight="1"/>
+    <row r="702" ht="16.5" customHeight="1"/>
+    <row r="703" ht="16.5" customHeight="1"/>
+    <row r="704" ht="16.5" customHeight="1"/>
+    <row r="705" ht="16.5" customHeight="1"/>
+    <row r="706" ht="16.5" customHeight="1"/>
+    <row r="707" ht="16.5" customHeight="1"/>
+    <row r="708" ht="16.5" customHeight="1"/>
+    <row r="709" ht="16.5" customHeight="1"/>
+    <row r="710" ht="16.5" customHeight="1"/>
+    <row r="711" ht="16.5" customHeight="1"/>
+    <row r="712" ht="16.5" customHeight="1"/>
+    <row r="713" ht="16.5" customHeight="1"/>
+    <row r="714" ht="16.5" customHeight="1"/>
+    <row r="715" ht="16.5" customHeight="1"/>
+    <row r="716" ht="16.5" customHeight="1"/>
+    <row r="717" ht="16.5" customHeight="1"/>
+    <row r="718" ht="16.5" customHeight="1"/>
+    <row r="719" ht="16.5" customHeight="1"/>
+    <row r="720" ht="16.5" customHeight="1"/>
+    <row r="721" ht="16.5" customHeight="1"/>
+    <row r="722" ht="16.5" customHeight="1"/>
+    <row r="723" ht="16.5" customHeight="1"/>
+    <row r="724" ht="16.5" customHeight="1"/>
+    <row r="725" ht="16.5" customHeight="1"/>
+    <row r="726" ht="16.5" customHeight="1"/>
+    <row r="727" ht="16.5" customHeight="1"/>
+    <row r="728" ht="16.5" customHeight="1"/>
+    <row r="729" ht="16.5" customHeight="1"/>
+    <row r="730" ht="16.5" customHeight="1"/>
+    <row r="731" ht="16.5" customHeight="1"/>
+    <row r="732" ht="16.5" customHeight="1"/>
+    <row r="733" ht="16.5" customHeight="1"/>
+    <row r="734" ht="16.5" customHeight="1"/>
+    <row r="735" ht="16.5" customHeight="1"/>
+    <row r="736" ht="16.5" customHeight="1"/>
+    <row r="737" ht="16.5" customHeight="1"/>
+    <row r="738" ht="16.5" customHeight="1"/>
+    <row r="739" ht="16.5" customHeight="1"/>
+    <row r="740" ht="16.5" customHeight="1"/>
+    <row r="741" ht="16.5" customHeight="1"/>
+    <row r="742" ht="16.5" customHeight="1"/>
+    <row r="743" ht="16.5" customHeight="1"/>
+    <row r="744" ht="16.5" customHeight="1"/>
+    <row r="745" ht="16.5" customHeight="1"/>
+    <row r="746" ht="16.5" customHeight="1"/>
+    <row r="747" ht="16.5" customHeight="1"/>
+    <row r="748" ht="16.5" customHeight="1"/>
+    <row r="749" ht="16.5" customHeight="1"/>
+    <row r="750" ht="16.5" customHeight="1"/>
+    <row r="751" ht="16.5" customHeight="1"/>
+    <row r="752" ht="16.5" customHeight="1"/>
+    <row r="753" ht="16.5" customHeight="1"/>
+    <row r="754" ht="16.5" customHeight="1"/>
+    <row r="755" ht="16.5" customHeight="1"/>
+    <row r="756" ht="16.5" customHeight="1"/>
+    <row r="757" ht="16.5" customHeight="1"/>
+    <row r="758" ht="16.5" customHeight="1"/>
+    <row r="759" ht="16.5" customHeight="1"/>
+    <row r="760" ht="16.5" customHeight="1"/>
+    <row r="761" ht="16.5" customHeight="1"/>
+    <row r="762" ht="16.5" customHeight="1"/>
+    <row r="763" ht="16.5" customHeight="1"/>
+    <row r="764" ht="16.5" customHeight="1"/>
+    <row r="765" ht="16.5" customHeight="1"/>
+    <row r="766" ht="16.5" customHeight="1"/>
+    <row r="767" ht="16.5" customHeight="1"/>
+    <row r="768" ht="16.5" customHeight="1"/>
+    <row r="769" ht="16.5" customHeight="1"/>
+    <row r="770" ht="16.5" customHeight="1"/>
+    <row r="771" ht="16.5" customHeight="1"/>
+    <row r="772" ht="16.5" customHeight="1"/>
+    <row r="773" ht="16.5" customHeight="1"/>
+    <row r="774" ht="16.5" customHeight="1"/>
+    <row r="775" ht="16.5" customHeight="1"/>
+    <row r="776" ht="16.5" customHeight="1"/>
+    <row r="777" ht="16.5" customHeight="1"/>
+    <row r="778" ht="16.5" customHeight="1"/>
+    <row r="779" ht="16.5" customHeight="1"/>
+    <row r="780" ht="16.5" customHeight="1"/>
+    <row r="781" ht="16.5" customHeight="1"/>
+    <row r="782" ht="16.5" customHeight="1"/>
+    <row r="783" ht="16.5" customHeight="1"/>
+    <row r="784" ht="16.5" customHeight="1"/>
+    <row r="785" ht="16.5" customHeight="1"/>
+    <row r="786" ht="16.5" customHeight="1"/>
+    <row r="787" ht="16.5" customHeight="1"/>
+    <row r="788" ht="16.5" customHeight="1"/>
+    <row r="789" ht="16.5" customHeight="1"/>
+    <row r="790" ht="16.5" customHeight="1"/>
+    <row r="791" ht="16.5" customHeight="1"/>
+    <row r="792" ht="16.5" customHeight="1"/>
+    <row r="793" ht="16.5" customHeight="1"/>
+    <row r="794" ht="16.5" customHeight="1"/>
+    <row r="795" ht="16.5" customHeight="1"/>
+    <row r="796" ht="16.5" customHeight="1"/>
+    <row r="797" ht="16.5" customHeight="1"/>
+    <row r="798" ht="16.5" customHeight="1"/>
+    <row r="799" ht="16.5" customHeight="1"/>
+    <row r="800" ht="16.5" customHeight="1"/>
+    <row r="801" ht="16.5" customHeight="1"/>
+    <row r="802" ht="16.5" customHeight="1"/>
+    <row r="803" ht="16.5" customHeight="1"/>
+    <row r="804" ht="16.5" customHeight="1"/>
+    <row r="805" ht="16.5" customHeight="1"/>
+    <row r="806" ht="16.5" customHeight="1"/>
+    <row r="807" ht="16.5" customHeight="1"/>
+    <row r="808" ht="16.5" customHeight="1"/>
+    <row r="809" ht="16.5" customHeight="1"/>
+    <row r="810" ht="16.5" customHeight="1"/>
+    <row r="811" ht="16.5" customHeight="1"/>
+    <row r="812" ht="16.5" customHeight="1"/>
+    <row r="813" ht="16.5" customHeight="1"/>
+    <row r="814" ht="16.5" customHeight="1"/>
+    <row r="815" ht="16.5" customHeight="1"/>
+    <row r="816" ht="16.5" customHeight="1"/>
+    <row r="817" ht="16.5" customHeight="1"/>
+    <row r="818" ht="16.5" customHeight="1"/>
+    <row r="819" ht="16.5" customHeight="1"/>
+    <row r="820" ht="16.5" customHeight="1"/>
+    <row r="821" ht="16.5" customHeight="1"/>
+    <row r="822" ht="16.5" customHeight="1"/>
+    <row r="823" ht="16.5" customHeight="1"/>
+    <row r="824" ht="16.5" customHeight="1"/>
+    <row r="825" ht="16.5" customHeight="1"/>
+    <row r="826" ht="16.5" customHeight="1"/>
+    <row r="827" ht="16.5" customHeight="1"/>
+    <row r="828" ht="16.5" customHeight="1"/>
+    <row r="829" ht="16.5" customHeight="1"/>
+    <row r="830" ht="16.5" customHeight="1"/>
+    <row r="831" ht="16.5" customHeight="1"/>
+    <row r="832" ht="16.5" customHeight="1"/>
+    <row r="833" ht="16.5" customHeight="1"/>
+    <row r="834" ht="16.5" customHeight="1"/>
+    <row r="835" ht="16.5" customHeight="1"/>
+    <row r="836" ht="16.5" customHeight="1"/>
+    <row r="837" ht="16.5" customHeight="1"/>
+    <row r="838" ht="16.5" customHeight="1"/>
+    <row r="839" ht="16.5" customHeight="1"/>
+    <row r="840" ht="16.5" customHeight="1"/>
+    <row r="841" ht="16.5" customHeight="1"/>
+    <row r="842" ht="16.5" customHeight="1"/>
+    <row r="843" ht="16.5" customHeight="1"/>
+    <row r="844" ht="16.5" customHeight="1"/>
+    <row r="845" ht="16.5" customHeight="1"/>
+    <row r="846" ht="16.5" customHeight="1"/>
+    <row r="847" ht="16.5" customHeight="1"/>
+    <row r="848" ht="16.5" customHeight="1"/>
+    <row r="849" ht="16.5" customHeight="1"/>
+    <row r="850" ht="16.5" customHeight="1"/>
+    <row r="851" ht="16.5" customHeight="1"/>
+    <row r="852" ht="16.5" customHeight="1"/>
+    <row r="853" ht="16.5" customHeight="1"/>
+    <row r="854" ht="16.5" customHeight="1"/>
+    <row r="855" ht="16.5" customHeight="1"/>
+    <row r="856" ht="16.5" customHeight="1"/>
+    <row r="857" ht="16.5" customHeight="1"/>
+    <row r="858" ht="16.5" customHeight="1"/>
+    <row r="859" ht="16.5" customHeight="1"/>
+    <row r="860" ht="16.5" customHeight="1"/>
+    <row r="861" ht="16.5" customHeight="1"/>
+    <row r="862" ht="16.5" customHeight="1"/>
+    <row r="863" ht="16.5" customHeight="1"/>
+    <row r="864" ht="16.5" customHeight="1"/>
+    <row r="865" ht="16.5" customHeight="1"/>
+    <row r="866" ht="16.5" customHeight="1"/>
+    <row r="867" ht="16.5" customHeight="1"/>
+    <row r="868" ht="16.5" customHeight="1"/>
+    <row r="869" ht="16.5" customHeight="1"/>
+    <row r="870" ht="16.5" customHeight="1"/>
+    <row r="871" ht="16.5" customHeight="1"/>
+    <row r="872" ht="16.5" customHeight="1"/>
+    <row r="873" ht="16.5" customHeight="1"/>
+    <row r="874" ht="16.5" customHeight="1"/>
+    <row r="875" ht="16.5" customHeight="1"/>
+    <row r="876" ht="16.5" customHeight="1"/>
+    <row r="877" ht="16.5" customHeight="1"/>
+    <row r="878" ht="16.5" customHeight="1"/>
+    <row r="879" ht="16.5" customHeight="1"/>
+    <row r="880" ht="16.5" customHeight="1"/>
+    <row r="881" ht="16.5" customHeight="1"/>
+    <row r="882" ht="16.5" customHeight="1"/>
+    <row r="883" ht="16.5" customHeight="1"/>
+    <row r="884" ht="16.5" customHeight="1"/>
+    <row r="885" ht="16.5" customHeight="1"/>
+    <row r="886" ht="16.5" customHeight="1"/>
+    <row r="887" ht="16.5" customHeight="1"/>
+    <row r="888" ht="16.5" customHeight="1"/>
+    <row r="889" ht="16.5" customHeight="1"/>
+    <row r="890" ht="16.5" customHeight="1"/>
+    <row r="891" ht="16.5" customHeight="1"/>
+    <row r="892" ht="16.5" customHeight="1"/>
+    <row r="893" ht="16.5" customHeight="1"/>
+    <row r="894" ht="16.5" customHeight="1"/>
+    <row r="895" ht="16.5" customHeight="1"/>
+    <row r="896" ht="16.5" customHeight="1"/>
+    <row r="897" ht="16.5" customHeight="1"/>
+    <row r="898" ht="16.5" customHeight="1"/>
+    <row r="899" ht="16.5" customHeight="1"/>
+    <row r="900" ht="16.5" customHeight="1"/>
+    <row r="901" ht="16.5" customHeight="1"/>
+    <row r="902" ht="16.5" customHeight="1"/>
+    <row r="903" ht="16.5" customHeight="1"/>
+    <row r="904" ht="16.5" customHeight="1"/>
+    <row r="905" ht="16.5" customHeight="1"/>
+    <row r="906" ht="16.5" customHeight="1"/>
+    <row r="907" ht="16.5" customHeight="1"/>
+    <row r="908" ht="16.5" customHeight="1"/>
+    <row r="909" ht="16.5" customHeight="1"/>
+    <row r="910" ht="16.5" customHeight="1"/>
+    <row r="911" ht="16.5" customHeight="1"/>
+    <row r="912" ht="16.5" customHeight="1"/>
+    <row r="913" ht="16.5" customHeight="1"/>
+    <row r="914" ht="16.5" customHeight="1"/>
+    <row r="915" ht="16.5" customHeight="1"/>
+    <row r="916" ht="16.5" customHeight="1"/>
+    <row r="917" ht="16.5" customHeight="1"/>
+    <row r="918" ht="16.5" customHeight="1"/>
+    <row r="919" ht="16.5" customHeight="1"/>
+    <row r="920" ht="16.5" customHeight="1"/>
+    <row r="921" ht="16.5" customHeight="1"/>
+    <row r="922" ht="16.5" customHeight="1"/>
+    <row r="923" ht="16.5" customHeight="1"/>
+    <row r="924" ht="16.5" customHeight="1"/>
+    <row r="925" ht="16.5" customHeight="1"/>
+    <row r="926" ht="16.5" customHeight="1"/>
+    <row r="927" ht="16.5" customHeight="1"/>
+    <row r="928" ht="16.5" customHeight="1"/>
+    <row r="929" ht="16.5" customHeight="1"/>
+    <row r="930" ht="16.5" customHeight="1"/>
+    <row r="931" ht="16.5" customHeight="1"/>
+    <row r="932" ht="16.5" customHeight="1"/>
+    <row r="933" ht="16.5" customHeight="1"/>
+    <row r="934" ht="16.5" customHeight="1"/>
+    <row r="935" ht="16.5" customHeight="1"/>
+    <row r="936" ht="16.5" customHeight="1"/>
+    <row r="937" ht="16.5" customHeight="1"/>
+    <row r="938" ht="16.5" customHeight="1"/>
+    <row r="939" ht="16.5" customHeight="1"/>
+    <row r="940" ht="16.5" customHeight="1"/>
+    <row r="941" ht="16.5" customHeight="1"/>
+    <row r="942" ht="16.5" customHeight="1"/>
+    <row r="943" ht="16.5" customHeight="1"/>
+    <row r="944" ht="16.5" customHeight="1"/>
+    <row r="945" ht="16.5" customHeight="1"/>
+    <row r="946" ht="16.5" customHeight="1"/>
+    <row r="947" ht="16.5" customHeight="1"/>
+    <row r="948" ht="16.5" customHeight="1"/>
+    <row r="949" ht="16.5" customHeight="1"/>
+    <row r="950" ht="16.5" customHeight="1"/>
+    <row r="951" ht="16.5" customHeight="1"/>
+    <row r="952" ht="16.5" customHeight="1"/>
+    <row r="953" ht="16.5" customHeight="1"/>
+    <row r="954" ht="16.5" customHeight="1"/>
+    <row r="955" ht="16.5" customHeight="1"/>
+    <row r="956" ht="16.5" customHeight="1"/>
+    <row r="957" ht="16.5" customHeight="1"/>
+    <row r="958" ht="16.5" customHeight="1"/>
+    <row r="959" ht="16.5" customHeight="1"/>
+    <row r="960" ht="16.5" customHeight="1"/>
+    <row r="961" ht="16.5" customHeight="1"/>
+    <row r="962" ht="16.5" customHeight="1"/>
+    <row r="963" ht="16.5" customHeight="1"/>
+    <row r="964" ht="16.5" customHeight="1"/>
+    <row r="965" ht="16.5" customHeight="1"/>
+    <row r="966" ht="16.5" customHeight="1"/>
+    <row r="967" ht="16.5" customHeight="1"/>
+    <row r="968" ht="16.5" customHeight="1"/>
+    <row r="969" ht="16.5" customHeight="1"/>
+    <row r="970" ht="16.5" customHeight="1"/>
+    <row r="971" ht="16.5" customHeight="1"/>
+    <row r="972" ht="16.5" customHeight="1"/>
+    <row r="973" ht="16.5" customHeight="1"/>
+    <row r="974" ht="16.5" customHeight="1"/>
+    <row r="975" ht="16.5" customHeight="1"/>
+    <row r="976" ht="16.5" customHeight="1"/>
+    <row r="977" ht="16.5" customHeight="1"/>
+    <row r="978" ht="16.5" customHeight="1"/>
+    <row r="979" ht="16.5" customHeight="1"/>
+    <row r="980" ht="16.5" customHeight="1"/>
+    <row r="981" ht="16.5" customHeight="1"/>
+    <row r="982" ht="16.5" customHeight="1"/>
+    <row r="983" ht="16.5" customHeight="1"/>
+    <row r="984" ht="16.5" customHeight="1"/>
+    <row r="985" ht="16.5" customHeight="1"/>
+    <row r="986" ht="16.5" customHeight="1"/>
+    <row r="987" ht="16.5" customHeight="1"/>
+    <row r="988" ht="16.5" customHeight="1"/>
+    <row r="989" ht="16.5" customHeight="1"/>
+    <row r="990" ht="16.5" customHeight="1"/>
+    <row r="991" ht="16.5" customHeight="1"/>
+    <row r="992" ht="16.5" customHeight="1"/>
+    <row r="993" ht="16.5" customHeight="1"/>
+    <row r="994" ht="16.5" customHeight="1"/>
+    <row r="995" ht="16.5" customHeight="1"/>
+    <row r="996" ht="16.5" customHeight="1"/>
+    <row r="997" ht="16.5" customHeight="1"/>
+    <row r="998" ht="16.5" customHeight="1"/>
+    <row r="999" ht="16.5" customHeight="1"/>
+    <row r="1000" ht="16.5" customHeight="1"/>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+  </mergeCells>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="2.38"/>
+    <col customWidth="1" min="2" max="2" width="14.38"/>
+    <col customWidth="1" min="3" max="3" width="38.88"/>
+    <col customWidth="1" min="4" max="5" width="28.5"/>
+    <col customWidth="1" min="6" max="6" width="4.88"/>
+    <col customWidth="1" min="7" max="26" width="7.63"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="12.75" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" ht="27.75" customHeight="1">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" ht="27.75" customHeight="1">
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" ht="27.75" customHeight="1">
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" ht="27.75" customHeight="1">
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" ht="27.75" customHeight="1">
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" ht="372.0" customHeight="1">
+      <c r="B7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
     </row>
     <row r="8" ht="16.5" customHeight="1"/>
     <row r="9" ht="16.5" customHeight="1"/>

</xml_diff>